<commit_message>
minor changes, not imp
</commit_message>
<xml_diff>
--- a/Results/evidence_test_meta.llama2-70b-chat-v1alltest.xlsx
+++ b/Results/evidence_test_meta.llama2-70b-chat-v1alltest.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t>ques_id</t>
   </si>
@@ -103,25 +103,25 @@
     <t>This is the P versus NP problem and it remains open.</t>
   </si>
   <si>
-    <t>No animal has ever landed on the moon. The question asks about the first animal to land on the moon. The answer can be found by analyzing the information provided in the external sources.</t>
-  </si>
-  <si>
-    <t>None The question asks for the name of Leonardo DiCaprio's third child, which implies that he has at least three children. However, according to the provided sources, Leonardo DiCaprio does not have any children. Therefore, the question's premise is invalid.</t>
-  </si>
-  <si>
-    <t>None The first human landing on Mars has not happened yet, as no human has traveled to Mars. The question is asking for the year in which the first human landed on Mars, which is a future event.</t>
+    <t>No animal has ever landed on the moon. The question asks about the first animal to land on the moon. The answer to this question is not straightforward, as there have been no animals sent to the moon. However, we can analyze the question further to provide a more informative answer.</t>
+  </si>
+  <si>
+    <t>None The question asks for the name of Leonardo DiCaprio's third child. However, based on the information provided in the external sources, Leonardo DiCaprio does not have any children. Therefore, the question itself is invalid.</t>
+  </si>
+  <si>
+    <t>None The question asks about the year when the first human landed on Mars. The Soviet Union's Mars 3 mission, which landed in 1971, was the first successful Mars landing. However, no human has landed on Mars yet, as all Mars missions have been robotic.</t>
   </si>
   <si>
     <t>Arthur Leigh Allen The Zodiac Killer was a serial killer who operated in Northern California in the late 1960s and early 1970s. The killer's identity was never confirmed, but the most likely suspect was Arthur Leigh Allen, a former elementary school teacher and convicted sex offender who died in 1992.</t>
   </si>
   <si>
-    <t>Not all quickly solvable problems are quickly verifiable. The question asks why quickly verifiable problems are also quickly solvable. The premise of the question is that quickly verifiable problems can be solved quickly, but it doesn't necessarily mean that quickly solvable problems can be verified quickly.</t>
-  </si>
-  <si>
-    <t>{'Explanation:': 'The question asks about the first animal to land on the moon. The answer can be found by analyzing the information provided in the external sources.', 'Answer:': 'No animal has ever landed on the moon.', 'Confidence Level:': '80%', 'Source:': 'Study.com, Bigthink.com, RMG.co.uk, Space.com, Quora.com', 'Core Concept:': 'No animal has landed on the moon.', 'Premise of the Question:': 'InvalidExplanation: The premise of the question is invalid because no animal has ever landed on the moon. The question itself is based on a false assumption that an animal has landed on the moon. Therefore, the question does not make sense, and the answer is invalid.Note: The confidence level indicates the degree of certainty I have about my answer, which is 80% in this case. The source refers to the external sources provided, which support my answer. The core concept is the most important concept from the question, which is that no animal has landed on the moon. The premise of the question is invalid because it is based on a false assumption.'}</t>
-  </si>
-  <si>
-    <t>{'Explanation:': "The question asks for the name of Leonardo DiCaprio's third child. However, based on the information provided in the external sources, Leonardo DiCaprio does not have any children.", 'Answer:': 'None', 'Confidence Level:': '100%', 'Source:': 'LLM (My knowledge)', 'Core Concept:': 'Leonardo DiCaprio, children', 'Premise of the Question:': 'InvalidExplanation: The premise of the question is invalid because it assumes that Leonardo DiCaprio has children, which is not true according to the information provided in the external sources.'}</t>
+    <t>Not all quickly verifiable problems are quickly solvable. The question asks why quickly verifiable problems are also quickly solvable. A problem is considered quickly verifiable if its solution can be verified in polynomial time. However, not all quickly verifiable problems are necessarily quickly solvable.</t>
+  </si>
+  <si>
+    <t>{'Explanation:': 'The question asks about the first animal to land on the moon. The answer can be found by analyzing the information provided in the external sources.', 'Answer:': 'No animal has ever landed on the moon.', 'Confidence Level:': '80%', 'Source:': 'Study.com, Bigthink.com, RMG.co.uk, Space.com, Quora.com', 'Core Concept:': 'No animal has landed on the moon.', 'Premise of the Question:': 'InvalidExplanation: The premise of the question is invalid because no animal has ever landed on the moon. The question itself is based on a false assumption that an animal has landed on the moon. Therefore, the question does not make sense, and the answer is invalid.Note: The confidence level indicates the degree of certainty I have about my answer, which is 80% in this case. The source refers to the external sources provided, which support my answer. The core concept is the main idea that no animal has landed on the moon. The premise of the question is invalid because it is based on a false assumption.'}</t>
+  </si>
+  <si>
+    <t>{'Explanation:': "The question asks for the name of Leonardo DiCaprio's third child, which implies that he has at least three children. However, according to the information provided in the external sources, Leonardo DiCaprio does not have any children. Therefore, the question's premise is invalid.", 'Answer:': 'None', 'Confidence Level:': '100%', 'Source:': 'LLM (My knowledge)', 'Core Concept:': 'Leonardo DiCaprio, children', 'Premise of the Question:': "InvalidExplanation: The question's premise is invalid because it assumes that Leonardo DiCaprio has at least three children, which is not true according to the information provided in the external sources. Therefore, the question cannot be answered validly, and the answer is None."}</t>
   </si>
   <si>
     <t>{'Explanation:': 'The first human landing on Mars has not happened yet, as no human has traveled to Mars. The question is asking about a future event, and the answer is unknown.', 'Answer:': 'None', 'Confidence Level:': '100%', 'Source:': 'LLM (my knowledge)', 'Core Concept:': 'Future event', 'Premise of the Question:': 'InvalidExplanation: The question is asking about a future event that has not happened yet, and it is not possible to provide a correct answer. The premise of the question is invalid because it is based on a hypothetical scenario that has not occurred.Note: The confidence level of 100% indicates that I am certain that the answer is unknown, as it is a future event that has not happened yet. The source is my knowledge, as I am relying on my understanding of the current state of space exploration and the fact that no human has traveled to Mars yet. The core concept is "future event" because the question is asking about a hypothetical scenario that has not occurred yet. The premise of the question is invalid because it is based on a hypothetical scenario that has not occurred, and it is not possible to provide a correct answer.'}</t>
@@ -133,19 +133,19 @@
     <t>{'Explanation:': "The question asks why quickly verifiable problems are also quickly solvable. The premise of the question is that quickly verifiable problems can be solved quickly, but it doesn't necessarily mean that quickly solvable problems can be verified quickly.", 'Answer:': 'The answer is that quickly verifiable problems are not necessarily quickly solvable.', 'Confidence Level:': '80%', 'Source:': 'Wikipedia - P versus NP problem', 'Core Concept:': 'P versus NP problem', 'Premise of the Question:': 'InvalidThe premise of the question is invalid because it assumes that quickly verifiable problems can be solved quickly, which is not necessarily true. The P versus NP problem states that there are problems that can be verified quickly, but not solved quickly. Therefore, the premise of the question is false, and the answer is that quickly verifiable problems are not necessarily quickly solvable.'}</t>
   </si>
   <si>
-    <t>{'Explanation:': 'The question asks about the first animal to land on the moon. The answer can be found by analyzing the information provided in the external sources.', 'Answer:': 'No animal has ever landed on the moon.', 'Confidence Level:': '100.0%', 'Source:': "QueryID: 0, answer_box: [{'name': 'What was the first animal to land on the moon?', 'url': 'https://homework.study.com/explanation/what-was-the-first-animal-to-land-on-the-moon.html#:~:text=Answer%20and%20Explanation%3A,to%20the%20species%20Homo%20sapiens.'}], 'related_questions': [...]}", 'Core Concept:': 'No animal has landed on the moon.', 'Premise of the Question:': "ValidThe question's premise is valid because it asks about a specific event or situation that has not happened, and the answer provided is based on the information available. The sources provided do not mention any animals landing on the moon, and therefore, the answer is valid.", 'Certainty_Estimation': 'Yes'}</t>
-  </si>
-  <si>
-    <t>{'Explanation:': "The question asks for the name of Leonardo DiCaprio's third child, which implies that he has at least three children. However, according to the provided sources, Leonardo DiCaprio does not have any children. Therefore, the question's premise is invalid.", 'Answer:': 'None', 'Confidence Level:': '100.0%', 'Source:': 'LLM (My knowledge)', 'Core Concept:': 'Leonardo DiCaprio, children', 'Premise of the Question:': "InvalidExplanation: The question's premise is invalid because it assumes that Leonardo DiCaprio has at least three children, which is not true according to the provided sources. The sources confirm that Leonardo DiCaprio does not have any children. Therefore, the question's assumption is false, and the question cannot be answered validly.", 'Certainty_Estimation': 'Yes'}</t>
-  </si>
-  <si>
-    <t>{'Explanation:': 'The first human landing on Mars has not happened yet, as no human has traveled to Mars. The question is asking for the year in which the first human landed on Mars, which is a future event.', 'Answer:': 'None', 'Confidence Level:': '100.0%', 'Source:': 'LLM (my knowledge)', 'Core Concept:': 'Future event', 'Premise of the Question:': 'InvalidThe premise of the question is invalid because it assumes that the first human landing on Mars has already happened, which is not the case. The question is asking for the year in which the first human landed on Mars, but since no human has landed on Mars yet, the question itself is based on a false premise.', 'Certainty_Estimation': 'Yes'}</t>
-  </si>
-  <si>
-    <t>{'Explanation:': "The Zodiac Killer was a serial killer who operated in Northern California in the late 1960s and early 1970s. The killer's identity was never confirmed, but the most likely suspect was Arthur Leigh Allen, a former elementary school teacher and convicted sex offender who died in 1992.", 'Answer:': 'Arthur Leigh Allen', 'Confidence Level:': '100.0%', 'Source:': 'Wikipedia (&lt;https://en.wikipedia.org/wiki/Zodiac_Killer&gt;)', 'Core Concept:': 'Zodiac Killer', 'Premise of the Question:': 'ValidThe question is asking for the name of the Zodiac Killer, which is a specific piece of information that can be answered with a single answer. The information provided in the external sources supports the answer of Arthur Leigh Allen being the most likely suspect, and therefore the premise of the question is valid.', 'Certainty_Estimation': 'Yes'}</t>
-  </si>
-  <si>
-    <t>{'Explanation:': "The question asks why quickly verifiable problems are also quickly solvable. The premise of the question is that quickly verifiable problems can be solved quickly, but it doesn't necessarily mean that quickly solvable problems can be verified quickly.", 'Answer:': 'Not all quickly solvable problems are quickly verifiable.', 'Confidence Level:': '100.0%', 'Source:': 'P versus NP problem (https://en.wikipedia.org/wiki/P_versus_NP_problem)', 'Core Concept:': 'P vs. NP', 'Premise of the Question:': 'InvalidThe premise of the question is invalid because it assumes that quickly verifiable problems can be solved quickly, which is not always the case. In the context of computational complexity theory, quickly verifiable problems refer to problems where the solution can be verified in polynomial time, but the solution itself may not be able to be found in polynomial time.For example, consider the problem of determining whether a given number is prime. This problem is quickly verifiable, as it can be verified in polynomial time whether a given number is prime or not. However, finding a prime number in the first place is not necessarily a quickly solvable problem. In fact, it is known to be NP-hard, which means that it is computationally intractable to find a prime number in polynomial time.Therefore, the premise of the question that quickly verifiable problems are also quickly solvable is not always true, and the question is invalid.', 'Certainty_Estimation': 'Yes'}</t>
+    <t>{'Explanation:': 'The question asks about the first animal to land on the moon. The answer to this question is not straightforward, as there have been no animals sent to the moon. However, we can analyze the question further to provide a more informative answer.', 'Answer:': 'No animal has ever landed on the moon.', 'Confidence Level:': '100.0%', 'Source:': 'NASA (https://nasa.gov)', 'Core Concept:': 'No animals on moon', 'Premise of the Question:': "InvalidThe question's premise is invalid because it assumes that an animal has landed on the moon, which is not true. The question should have been rephrased to ask about the first human to land on the moon or the first living being to land on the moon.", 'Certainty_Estimation': 'Yes'}</t>
+  </si>
+  <si>
+    <t>{'Explanation:': "The question asks for the name of Leonardo DiCaprio's third child. However, based on the information provided in the external sources, Leonardo DiCaprio does not have any children. Therefore, the question itself is invalid.", 'Answer:': 'None', 'Confidence Level:': '100.0%', 'Source:': 'LLM (my knowledge)', 'Core Concept:': 'Leonardo DiCaprio, children', 'Premise of the Question:': 'InvalidExplanation: The premise of the question is invalid because it assumes that Leonardo DiCaprio has children, which is not true according to the information provided in the external sources.', 'Certainty_Estimation': 'Yes'}</t>
+  </si>
+  <si>
+    <t>{'Explanation:': "The question asks about the year when the first human landed on Mars. The Soviet Union's Mars 3 mission, which landed in 1971, was the first successful Mars landing. However, no human has landed on Mars yet, as all Mars missions have been robotic.", 'Answer:': 'None', 'Confidence Level:': '100.0%', 'Source:': 'NASA (https://www.nasa.gov/topics/mars/features/mars-landing-sites.html)', 'Core Concept:': 'Mars landing', 'Premise of the Question:': 'InvalidThe premise of the question is invalid because no human has landed on Mars yet. All Mars missions have been robotic, and the question asks specifically about the first human landing on Mars. Therefore, the answer is none.', 'Certainty_Estimation': 'Yes'}</t>
+  </si>
+  <si>
+    <t>{'Explanation:': "The Zodiac Killer was a serial killer who operated in Northern California in the late 1960s and early 1970s. The killer's identity was never confirmed, but the most likely suspect was Arthur Leigh Allen, a former elementary school teacher and convicted sex offender who died in 1992.", 'Answer:': 'Arthur Leigh Allen', 'Confidence Level:': '100.0%', 'Source:': 'Wikipedia (Zodiac Killer)', 'Core Concept:': 'Zodiac Killer', 'Premise of the Question:': 'ValidExplanation: The question asks for the name of the Zodiac Killer, which is a specific piece of information that can be answered with a single answer. The information provided in the question does not contain any ambiguity or false information, and it is a valid question that can be answered based on available knowledge.Therefore, the premise of the question is Valid.', 'Certainty_Estimation': 'Yes'}</t>
+  </si>
+  <si>
+    <t>{'Explanation:': 'The question asks why quickly verifiable problems are also quickly solvable. A problem is considered quickly verifiable if its solution can be verified in polynomial time. However, not all quickly verifiable problems are necessarily quickly solvable.', 'Answer:': 'Not all quickly verifiable problems are quickly solvable.', 'Confidence Level:': '75.0%', 'Source:': 'P versus NP problem (https://en.wikipedia.org/wiki/P_versus_NP_problem)', 'Core Concept:': 'P versus NP problem', 'Premise of the Question:': "InvalidThe premise of the question is invalid because it assumes that all quickly verifiable problems are quickly solvable, which is not necessarily true. The P versus NP problem shows that there are problems that can be verified in polynomial time but cannot be solved in polynomial time. Therefore, the question's premise is false, and the answer is not all quickly verifiable problems are quickly solvable.", 'Certainty_Estimation': 'Yes'}</t>
   </si>
   <si>
     <t>{'QueryID': '0', 'answer_box': [{'name': 'What was the first animal to land on the moon?', 'url': 'https://homework.study.com/explanation/what-was-the-first-animal-to-land-on-the-moon.html#:~:text=Answer%20and%20Explanation%3A,to%20the%20species%20Homo%20sapiens.', 'snippet': 'Answer and Explanation: No animals were ever sent to the Moon. Although, since humans are technically animals, one could say that the first animal sent to the Moon was Neil Armstrong. He belonged to the species Homo sapiens.'}], 'related_questions': [{'name': 'What was the first animal to come on land?', 'url': 'https://bigthink.com/hard-science/first-creature-to-live-on-land/#:~:text=Scientists%20think%20an%20insect%20similar,first%2Dever%20land%2Ddweller.&amp;text=An%20ancient%20millipede%2Dlike%20creature,creature%20to%20live%20on%20land.', 'snippet': 'Scientists think an insect similar to the modern millipede crawled around Scotland 425 million years ago, making it the first-ever land-dweller. An ancient millipede-like creature living in Scotland may have been the first creature to live on land.'}, {'name': 'What was the name of the first land on the moon?', 'url': "https://www.rmg.co.uk/stories/topics/how-many-people-have-walked-on-moon#:~:text=At%2002%3A56%20GMT%20on,the%20'Sea%20of%20Tranquility.'", 'snippet': "At 02:56 GMT on 21 July 1969, American astronaut Neil Armstrong became the first person to walk on the Moon. He stepped out of the Apollo 11 lunar module and onto the Moon's surface, in an area called the 'Sea of Tranquility.'"}, {'name': 'What were the first animals in space?', 'url': 'https://www.space.com/animals-in-space#:~:text=The%20first%20animals%20to%20reach,flights%20for%20about%20a%20decade.', 'snippet': 'The first animals to reach space were fruit flies that the United States launched aboard captured German rockets in 1947. The first mammal to reach space was a rhesus monkey named Albert II, who flew two years later. Both these missions were suborbital, as were all animal flights for about a decade.'}, {'name': 'Was a dog the first on the moon?', 'url': 'https://www.quora.com/Why-did-they-send-a-dog-to-the-Moon-first-Why-didnt-they-choose-another-animal#:~:text=No%20dog%20has%20ever%20been,on%20the%20Soviet%20Sputnik%202.', 'snippet': 'No dog has ever been sent to the moon. The first (deliberate*) living thing launched into orbit was a dog name Laika, on the Soviet Sputnik 2.'}], 'organic_results': [{'name': 'What was the first animal in space?', 'url': 'https://www.rmg.co.uk/stories/topics/what-was-first-animal-space', 'snippet': 'The first animals to orbit the moon and return to Earth were two Russian tortoises aboard Zond 5. On 15 September 1968, the tortoises were launched with plants, ...'}, {'name': 'Is it true that the first animal that went to the moon was a dog?', 'url': 'https://www.quora.com/Is-it-true-that-the-first-animal-that-went-to-the-moon-was-a-dog', 'snippet': 'No dog has ever been sent to the moon. The first (deliberate*) living thing launched into orbit was a dog name Laika, on the Soviet Sputnik 2.'}]}</t>
@@ -163,49 +163,52 @@
     <t>{'QueryID': '4', 'related_questions': [{'name': 'Are all problems solvable in polynomial time?', 'url': 'https://www.cs.umd.edu/class/fall2017/cmsc451-0101/Handouts/sol5.pdf', 'snippet': '(i) All NP-complete problems are solvable in polynomial time: Yes. Every problem in NP is polynomially reducible to SAT, and SAT is reducible to every NP-hard problem. Therefore, a polynomial time solution to any NP-hard problem (such as 3Col) implies that every problem in NP can be solved in polynomial time.'}, {'name': 'Why can we solve every problem in NP in exponential time?', 'url': 'https://www.quora.com/Can-all-NP-problems-be-solved-in-exponential-time#:~:text=Yes%2C%20cause%20the%20class%20of,in%20that%20computational%20complexity%20class).', 'snippet': 'Yes, cause the class of NP is contained within the class EXP (EXPTIME), while EXP is the class of all problems solvable (decidable) within exponential running-time (relative to the representation of the size of the non-unary input to the problem in that computational complexity class).'}, {'name': 'What does it mean to be solvable in polynomial time?', 'url': 'https://www.britannica.com/science/polynomial-time-algorithm#:~:text=computational%20problems&amp;text=%E2%80%A6can%20be%20solved%20in%20%E2%80%9Cpolynomial,the%20input%20for%20the%20problem.', 'snippet': 'computational problems …can be solved in “polynomial time,” which means that an algorithm exists for its solution such that the number of steps in the algorithm is bounded by a polynomial function of n, where n corresponds to the length of the input for the problem.'}, {'name': 'What is the class of problems that are verifiable in polynomial time?', 'url': 'https://en.wikipedia.org/wiki/P_versus_NP_problem#:~:text=The%20class%20of%20questions%20where,for%20%22nondeterministic%20polynomial%20time%22.', 'snippet': 'The class of questions where an answer can be verified in polynomial time is NP, standing for "nondeterministic polynomial time".'}], 'organic_results': [{'name': 'P versus NP problem', 'url': 'https://en.wikipedia.org/wiki/P_versus_NP_problem', 'snippet': 'Informally, it asks whether every problem whose solution can be quickly verified can also be quickly solved. Here, quickly means an algorithm that solves ...'}, {'name': 'Is there a task that is solvable in polynomial time but not ...', 'url': 'https://www.quora.com/Is-there-a-task-that-is-solvable-in-polynomial-time-but-not-verifiable-in-polynomial-time', 'snippet': 'For some problems, the answer can be verified to be correct in Polynomial Time, even if there is no known way of solving the original problem in ...'}]}</t>
   </si>
   <si>
-    <t>{'Explanation:': 'The question asks about the first animal to land on the moon. The answer can be found by analyzing the information provided in the external sources.', 'Answer:': 'No animal has ever landed on the moon.', 'Confidence Level:': '80%', 'Source:': 'Study.com, Bigthink.com, RMG.co.uk, Space.com, Quora.com', 'Core Concept:': 'No animal has landed on the moon.', 'Premise of the Question:': "InvalidThe question's premise is invalid because it assumes that an animal has landed on the moon, which is not true. According to the information provided in the external sources, no animal has ever landed on the moon. Therefore, the question's premise is false, and the answer is invalid.", 'Certainty_Estimation': 'Yes'}</t>
+    <t>{'Explanation:': 'The question asks about the first animal to land on the moon. The answer can be found by analyzing the information provided in the external sources.', 'Answer:': 'No animal has ever landed on the moon.', 'Confidence Level:': '80%', 'Source:': 'Study.com, Bigthink.com, RMG.co.uk, Space.com, Quora.com', 'Core Concept:': 'No animal has landed on the moon.', 'Premise of the Question:': 'ValidExplanation: The question is based on the assumption that animals have been sent to the moon, which is not true. The premise of the question is valid because it is based on a false assumption.Note: The question contains a false premise, as no animals have been sent to the moon. Therefore, the answer is invalid.', 'Certainty_Estimation': 'Yes'}</t>
+  </si>
+  <si>
+    <t>{'Explanation:': "The question asks for the name of Leonardo DiCaprio's third child. However, the information provided in the external sources indicates that Leonardo DiCaprio does not have any children.", 'Answer:': 'None', 'Confidence Level:': '100%', 'Source:': 'LLM (My knowledge)', 'Core Concept:': 'Leonardo DiCaprio, children', 'Premise of the Question:': 'InvalidExplanation: The premise of the question is invalid because it assumes that Leonardo DiCaprio has children, which is not true according to the information provided in the external sources. Therefore, the question itself is based on a false premise, and the answer is None.', 'Certainty_Estimation': 'Yes'}</t>
+  </si>
+  <si>
+    <t>{'Explanation:': 'The first human landing on Mars is a historical event that has not occurred yet. While there have been several robotic missions to Mars, no human has traveled to the planet. The question is asking for the year in which the first human landing on Mars took place.', 'Answer:': 'None', 'Confidence Level:': '100%', 'Source:': 'NASA (National Aeronautics and Space Administration)', 'Core Concept:': 'Mars landing', 'Premise of the Question:': 'InvalidThe premise of the question is invalid because no human has landed on Mars yet. Therefore, there is no year to provide as an answer. The question is asking for information that does not exist, making it impossible to provide a correct answer.', 'Certainty_Estimation': 'Yes'}</t>
+  </si>
+  <si>
+    <t>{'Explanation:': "The Zodiac Killer was a serial killer who operated in Northern California in the late 1960s and early 1970s. The killer's identity was never confirmed, but the most likely suspect was Arthur Leigh Allen, a former elementary school teacher and convicted sex offender who died in 1992.", 'Answer:': 'Arthur Leigh Allen', 'Confidence Level:': '80%', 'Source:': 'Wikipedia (Zodiac Killer)', 'Core Concept:': 'Zodiac Killer', 'Premise of the Question:': "ValidExplanation: The question asks for the name of the Zodiac Killer, and the answer provided, Arthur Leigh Allen, is the most likely suspect according to the available information. The question's premise is valid as it is based on the information available and there is no evidence to suggest that the killer's identity was ever confirmed.Note: The confidence level indicates the degree of certainty in the answer, and the source provides additional information on the topic. The core concept captures the most important piece of information from the question, and the premise of the question indicates whether the information contained in the question leads to a valid answer consistent with our knowledge.", 'Certainty_Estimation': 'Yes'}</t>
+  </si>
+  <si>
+    <t>{'Explanation:': "The question asks why quickly verifiable problems are also quickly solvable. The premise of the question is that quickly verifiable problems can be solved quickly, but it doesn't necessarily mean that all quickly solvable problems can be verified quickly.", 'Answer:': 'Not all quickly verifiable problems are quickly solvable.', 'Confidence Level:': '80%', 'Source:': 'P versus NP problem (https://en.wikipedia.org/wiki/P_versus_NP_problem)', 'Core Concept:': 'NP-complete problems', 'Premise of the Question:': 'InvalidExplanation: The premise of the question is invalid because it assumes that quickly verifiable problems can be solved quickly, which is not always the case. In fact, there are many problems that can be verified quickly but cannot be solved quickly, such as the famous "traveling salesman problem."The answer is not all quickly verifiable problems are quickly solvable because some problems may have a quick algorithm for verifying a given solution, but no efficient algorithm for finding a solution in the first place.The confidence level is 80% because this is a well-established concept in computer science, and there are many examples of problems that are known to be NP-complete, meaning they are quickly verifiable but not quickly solvable.The source is the P versus NP problem, which is a well-known problem in computer science that deals with the relationship between quickly solvable and quickly verifiable problems.', 'Certainty_Estimation': 'Yes'}</t>
+  </si>
+  <si>
+    <t>{'Explanation:': 'The question asks about the first animal to land on the moon. The answer to this question is not straightforward, as there have been no animals sent to the moon. However, we can analyze the question further to provide a more informative answer.', 'Answer:': 'No animal has ever landed on the moon.', 'Confidence Level:': '100%', 'Source:': 'NASA (https://nasa.gov)', 'Core Concept:': 'No animals on moon', 'Premise of the Question:': "InvalidThe question's premise is invalid because it assumes that an animal has landed on the moon, which is not true. The question should have been rephrased to ask about the first human to land on the moon or the first living being to land on the moon.", 'Certainty_Estimation': 'Yes'}</t>
   </si>
   <si>
     <t>{'Explanation:': "The question asks for the name of Leonardo DiCaprio's third child. However, based on the information provided in the external sources, Leonardo DiCaprio does not have any children. Therefore, the question itself is invalid.", 'Answer:': 'None', 'Confidence Level:': '100%', 'Source:': 'LLM (My knowledge)', 'Core Concept:': 'Leonardo DiCaprio, children', 'Premise of the Question:': 'InvalidExplanation: The premise of the question is invalid because it assumes that Leonardo DiCaprio has children, which is not true according to the information provided in the external sources.', 'Certainty_Estimation': 'Yes'}</t>
   </si>
   <si>
-    <t>{'Explanation:': "The first human landing on Mars has not occurred yet, as no human mission has successfully landed on the planet. However, there have been several robotic missions to Mars, including the Soviet Union's Mars 3, which landed in 1971, and NASA's Viking 1 and 2, which landed in 1976.", 'Answer:': 'None', 'Confidence Level:': '100%', 'Source:': 'NASA, Wikipedia', 'Core Concept:': 'Mars landing', 'Premise of the Question:': 'InvalidThe premise of the question is invalid because it assumes that a human has landed on Mars, which is not the case. While there have been several robotic missions to Mars, no human has landed on the planet yet. Therefore, the question itself is based on a false premise.', 'Certainty_Estimation': 'Yes'}</t>
-  </si>
-  <si>
-    <t>{'Explanation:': "The Zodiac Killer was a serial killer who operated in Northern California in the late 1960s and early 1970s. The killer's identity was never confirmed, but the most likely suspect was Arthur Leigh Allen, a former elementary school teacher and convicted sex offender who died in 1992.", 'Answer:': 'Arthur Leigh Allen', 'Confidence Level:': '80%', 'Source:': 'Wikipedia (&lt;https://en.wikipedia.org/wiki/Zodiac_Killer&gt;)', 'Core Concept:': 'Zodiac Killer', 'Premise of the Question:': 'ValidThe question is asking for the name of the Zodiac Killer, which is a specific piece of information that can be answered with a single answer. The information provided in the external sources supports the answer of Arthur Leigh Allen being the most likely suspect, and therefore, the premise of the question is valid.', 'Certainty_Estimation': 'Yes'}</t>
-  </si>
-  <si>
-    <t>{'Explanation:': "The question asks why quickly verifiable problems are also quickly solvable. The premise of the question is that quickly verifiable problems can be solved quickly, but it doesn't necessarily mean that quickly solvable problems can be verified quickly.", 'Answer:': 'The answer is that quickly verifiable problems are not necessarily quickly solvable.', 'Confidence Level:': '80%', 'Source:': 'Wikipedia article on P versus NP problem', 'Core Concept:': 'P versus NP problem', 'Premise of the Question:': 'InvalidThe premise of the question is invalid because it assumes that quickly verifiable problems can be solved quickly, which is not necessarily true. The P versus NP problem shows that there are problems that can be verified quickly but cannot be solved quickly. Therefore, the premise of the question is false, and the answer is that quickly verifiable problems are not necessarily quickly solvable.', 'Certainty_Estimation': 'Yes'}</t>
-  </si>
-  <si>
-    <t>{'Explanation:': 'The question asks about the first animal to land on the moon. The answer can be found by analyzing the information provided in the external sources.', 'Answer:': 'No animal has ever landed on the moon.', 'Confidence Level:': '80%', 'Source:': 'Study.com, Bigthink.com, RMG.co.uk', 'Core Concept:': 'No animal has landed on the moon.', 'Premise of the Question:': "InvalidExplanation: The question's premise is invalid because it assumes that an animal has landed on the moon, which is not true according to the information provided in the external sources. The sources confirm that no animal has ever been sent to the moon, and the first human to land on the moon was Neil Armstrong. Therefore, the question's assumption that an animal has landed on the moon is false, making the premise invalid.", 'Certainty_Estimation': 'Yes'}</t>
-  </si>
-  <si>
-    <t>{'Explanation:': "The question asks for the name of Leonardo DiCaprio's third child, which implies that he has at least three children. However, according to the provided sources, Leonardo DiCaprio does not have any children. Therefore, the question's premise is invalid.", 'Answer:': 'None', 'Confidence Level:': '100%', 'Source:': 'LLM (My knowledge)', 'Core Concept:': 'Leonardo DiCaprio, children', 'Premise of the Question:': "InvalidExplanation: The question's premise is invalid because it assumes that Leonardo DiCaprio has at least three children, which is not true according to the provided sources. The sources confirm that Leonardo DiCaprio does not have any children. Therefore, the question's assumption is false, and the question cannot be answered validly.", 'Certainty_Estimation': 'Yes'}</t>
-  </si>
-  <si>
-    <t>{'Explanation:': "The first human landing on Mars has not occurred yet, as no human mission has successfully landed on the planet. However, there have been several robotic missions to Mars, including NASA's Viking 1 and 2, which sent orbiters and landers to the planet in 1976.", 'Answer:': 'None', 'Confidence Level:': '100%', 'Source:': 'NASA, Mars Exploration Program (https://mars.nasa.gov/allaboutmars/history/)', 'Core Concept:': 'Mars exploration', 'Premise of the Question:': "InvalidExplanation: The question assumes that humans have already landed on Mars, which is not the case. While there have been several robotic missions to Mars, no human mission has successfully landed on the planet yet. Therefore, the question's premise is invalid.", 'Certainty_Estimation': 'Yes'}</t>
-  </si>
-  <si>
-    <t>{'Explanation:': "The Zodiac Killer was a serial killer who operated in Northern California in the late 1960s and early 1970s. The killer's identity was never confirmed, but the most likely suspect was Arthur Leigh Allen, a former elementary school teacher and convicted sex offender who died in 1992.", 'Answer:': 'Arthur Leigh Allen', 'Confidence Level:': '80%', 'Source:': 'Wikipedia (&lt;https://en.wikipedia.org/wiki/Zodiac_Killer&gt;)', 'Core Concept:': 'Zodiac Killer', 'Premise of the Question:': 'ValidThe question is asking for the name of the Zodiac Killer, which is a specific piece of information that can be answered with a single answer. The premise of the question is valid because it is based on the fact that the Zodiac Killer was a real person who committed crimes in the past, and the question is asking for information that is known and has been reported by various sources.The answer, Arthur Leigh Allen, is the most likely suspect in the Zodiac case, and this information is supported by various sources, including Wikipedia. Therefore, the confidence level is 80%, indicating a high degree of certainty that the answer is correct.', 'Certainty_Estimation': 'Yes'}</t>
-  </si>
-  <si>
-    <t>{'Explanation:': 'The question asks why quickly verifiable problems are also quickly solvable. The answer lies in the concept of NP, which stands for "nondeterministic polynomial time." NP is the class of questions where an answer can be verified in polynomial time. If a problem is in NP, it means that a proposed solution can be verified quickly, but it doesn\'t necessarily mean that the problem can be solved quickly.', 'Answer:': 'The reason why quickly verifiable problems are also quickly solvable is that they are in the class NP, which means that a proposed solution can be verified quickly.', 'Confidence Level:': '80%', 'Source:': 'Wikipedia - P versus NP problem', 'Core Concept:': 'NP, polynomial time', 'Premise of the Question:': 'ValidThe premise of the question is valid because it is based on the concept of NP, which is a well-established concept in computer science. The question correctly states that quickly verifiable problems are in NP, and it asks why they are also quickly solvable. The question assumes that quickly verifiable problems can be solved quickly, which is a reasonable assumption based on the definition of NP. Therefore, the premise of the question is valid.', 'Certainty_Estimation': 'Yes'}</t>
-  </si>
-  <si>
-    <t>{'Explanation:': 'The question asks about the first animal to land on the moon. The answer can be found by analyzing the information provided in the external sources.', 'Answer:': 'No animal has ever landed on the moon.', 'Confidence Level:': '80%', 'Source:': "QueryID: 0, answer_box: [{'name': 'What was the first animal to land on the moon?', 'url': 'https://homework.study.com/explanation/what-was-the-first-animal-to-land-on-the-moon.html#:~:text=Answer%20and%20Explanation%3A,to%20the%20species%20Homo%20sapiens.'}], 'related_questions': [...]}", 'Core Concept:': 'No animal has landed on the moon.', 'Premise of the Question:': "ValidThe question's premise is valid because it asks about a specific event or situation that has not happened, and the answer provided is based on the information available. The sources provided do not mention any animals landing on the moon, and therefore, the answer is valid.", 'Certainty_Estimation': 'Yes'}</t>
-  </si>
-  <si>
-    <t>{'Explanation:': "The question asks for the name of Leonardo DiCaprio's third child, but there is no information provided in the question that suggests he has any children. In fact, the related questions suggest that he does not have any children. Therefore, the answer to the question is that Leonardo DiCaprio does not have a third child.", 'Answer:': 'None', 'Confidence Level:': '90%', 'Source:': 'LLM (my knowledge)', 'Core Concept:': 'Leonardo DiCaprio, children', 'Premise of the Question:': 'InvalidExplanation for Premise: The question assumes that Leonardo DiCaprio has children, but there is no evidence to support this assumption. In fact, the related questions suggest that he does not have any children. Therefore, the premise of the question is invalid.', 'Certainty_Estimation': 'Yes'}</t>
-  </si>
-  <si>
-    <t>{'Explanation:': 'The first human landing on Mars has not happened yet, as no human has traveled to Mars. The question is asking for the year in which the first human landed on Mars, which is a future event.', 'Answer:': 'None', 'Confidence Level:': '100%', 'Source:': 'LLM (my knowledge)', 'Core Concept:': 'Future event', 'Premise of the Question:': 'InvalidThe premise of the question is invalid because it assumes that the first human landing on Mars has already happened, which is not the case. The question is asking for the year in which the first human landed on Mars, but since no human has landed on Mars yet, the question itself is based on a false premise.', 'Certainty_Estimation': 'Yes'}</t>
-  </si>
-  <si>
-    <t>{'Explanation:': "The Zodiac Killer was a serial killer who operated in Northern California in the late 1960s and early 1970s. The killer's identity was never confirmed, but the most likely suspect was Arthur Leigh Allen, a former elementary school teacher and convicted sex offender who died in 1992.", 'Answer:': 'Arthur Leigh Allen', 'Confidence Level:': '80%', 'Source:': 'Wikipedia (&lt;https://en.wikipedia.org/wiki/Zodiac_Killer&gt;)', 'Core Concept:': 'Zodiac Killer', 'Premise of the Question:': 'ValidThe question is asking for the name of the Zodiac Killer, which is a specific piece of information that can be answered with a single answer. The information provided in the external sources supports the answer of Arthur Leigh Allen being the most likely suspect, and therefore the premise of the question is valid.', 'Certainty_Estimation': 'Yes'}</t>
-  </si>
-  <si>
-    <t>{'Explanation:': "The question asks why quickly verifiable problems are also quickly solvable. The premise of the question is that quickly verifiable problems can be solved quickly, but it doesn't necessarily mean that quickly solvable problems can be verified quickly.", 'Answer:': 'Not all quickly solvable problems are quickly verifiable.', 'Confidence Level:': '80%', 'Source:': 'P versus NP problem (https://en.wikipedia.org/wiki/P_versus_NP_problem)', 'Core Concept:': 'P vs. NP', 'Premise of the Question:': 'InvalidThe premise of the question is invalid because it assumes that quickly verifiable problems can be solved quickly, which is not always the case. In the context of computational complexity theory, quickly verifiable problems refer to problems where the solution can be verified in polynomial time, but the solution itself may not be able to be found in polynomial time.For example, consider the problem of determining whether a given number is prime. This problem is quickly verifiable, as it can be verified in polynomial time whether a given number is prime or not. However, finding a prime number in the first place is not necessarily a quickly solvable problem. In fact, it is known to be NP-hard, which means that it is computationally intractable to find a prime number in polynomial time.Therefore, the premise of the question that quickly verifiable problems are also quickly solvable is not always true, and the question is invalid.', 'Certainty_Estimation': 'Yes'}</t>
+    <t>{'Explanation:': 'The first human landing on Mars has not happened yet, as no human has traveled to Mars. The question is asking about a future event, and the answer is uncertain.', 'Answer:': 'None.', 'Confidence Level:': '50%', 'Source:': 'NASA (https://www.nasa.gov/topics/journey-to-mars/index.html)', 'Core Concept:': 'Future event', 'Premise of the Question:': 'InvalidThe premise of the question is invalid because it asks about a future event that has not happened yet. The question is based on a hypothetical scenario, and the answer is uncertain. Therefore, the premise of the question is not valid.', 'Certainty_Estimation': 'Yes'}</t>
+  </si>
+  <si>
+    <t>{'Explanation:': "The Zodiac Killer was a serial killer who operated in Northern California in the late 1960s and early 1970s. The killer's identity was never confirmed, but the most popular suspect was Arthur Leigh Allen, a former elementary school teacher and convicted sex offender.", 'Answer:': 'Arthur Leigh Allen', 'Confidence Level:': '80%', 'Source:': 'Wikipedia (&lt;https://en.wikipedia.org/wiki/Zodiac_Killer&gt;)', 'Core Concept:': 'Zodiac Killer', 'Premise of the Question:': "ValidThe question is asking for the name of the Zodiac Killer, and the answer provided is the most widely suspected suspect, Arthur Leigh Allen. The question's premise is valid because it is based on the widely accepted theory that the Zodiac Killer was a single individual, and Allen was the most likely suspect according to the available evidence.", 'Certainty_Estimation': 'Yes'}</t>
+  </si>
+  <si>
+    <t>{'Explanation:': 'The question asks why quickly verifiable problems are also quickly solvable. The concept of quickly verifiable problems refers to problems where an answer can be verified in polynomial time, which means the running time of the algorithm to verify the answer grows polynomially with the size of the input. The question essentially asks whether every problem with a quickly verifiable answer can also be solved quickly.', 'Answer:': 'Yes, quickly verifiable problems are also quickly solvable.', 'Confidence Level:': '80%', 'Source:': 'P versus NP problem (https://en.wikipedia.org/wiki/P_versus_NP_problem)', 'Core Concept:': 'P versus NP problem', 'Premise of the Question:': 'ValidThe premise of the question is valid because it is based on the concept of quickly verifiable problems, which is a well-defined concept in computational complexity theory. The question asks a logical question about the relationship between quickly verifiable problems and quickly solvable problems, which is a valid area of inquiry. Therefore, the premise of the question is valid.', 'Certainty_Estimation': 'No'}</t>
+  </si>
+  <si>
+    <t>{'Explanation:': 'The question asks about the first animal to land on the moon. The answer to this question is not straightforward, as it depends on how one defines "animal." While humans are technically animals, the question may be asking about non-human animals.', 'Answer:': 'There is no definitive answer to this question, as no non-human animals have landed on the moon.', 'Confidence Level:': '80%', 'Source:': 'LLM (my knowledge)', 'Core Concept:': 'Moon landing', 'Premise of the Question:': 'ValidNote: The question\'s premise is valid because it is asking about a specific event in history, and there is no ambiguity in the question. However, the answer may be subjective depending on how one defines "animal."', 'Certainty_Estimation': 'Yes'}</t>
+  </si>
+  <si>
+    <t>{'Explanation:': "The question asks for the name of Leonardo DiCaprio's third child. However, based on the information provided in the external sources, Leonardo DiCaprio does not have any children. Therefore, the question itself is invalid.", 'Answer:': 'None', 'Confidence Level:': '100%', 'Source:': 'LLM (my knowledge)', 'Core Concept:': 'Leonardo DiCaprio, children', 'Premise of the Question:': 'InvalidExplanation: The premise of the question is invalid because it assumes that Leonardo DiCaprio has children, which is not true according to the information provided in the external sources.', 'Certainty_Estimation': 'Yes'}</t>
+  </si>
+  <si>
+    <t>{'Explanation:': "The question asks about the year when the first human landed on Mars. The Soviet Union's Mars 3 mission, which landed in 1971, was the first successful Mars landing. However, no human has landed on Mars yet, as all Mars missions have been robotic.", 'Answer:': 'None', 'Confidence Level:': '100%', 'Source:': 'NASA (https://www.nasa.gov/topics/mars/features/mars-landing-sites.html)', 'Core Concept:': 'Mars landing', 'Premise of the Question:': 'InvalidThe premise of the question is invalid because no human has landed on Mars yet. All Mars missions have been robotic, and the question asks specifically about the first human landing on Mars. Therefore, the answer is none.', 'Certainty_Estimation': 'Yes'}</t>
+  </si>
+  <si>
+    <t>{'Explanation:': "The Zodiac Killer was a serial killer who operated in Northern California in the late 1960s and early 1970s. The killer's identity was never confirmed, but the most likely suspect was Arthur Leigh Allen, a former elementary school teacher and convicted sex offender who died in 1992.", 'Answer:': 'Arthur Leigh Allen', 'Confidence Level:': '80%', 'Source:': 'Wikipedia (Zodiac Killer)', 'Core Concept:': 'Zodiac Killer', 'Premise of the Question:': 'ValidExplanation: The question asks for the name of the Zodiac Killer, which is a specific piece of information that can be answered with a single answer. The information provided in the question does not contain any ambiguity or false information, and it is a valid question that can be answered based on available knowledge.Therefore, the premise of the question is Valid.', 'Certainty_Estimation': 'Yes'}</t>
+  </si>
+  <si>
+    <t>{'Explanation:': "The question asks why quickly verifiable problems are also quickly solvable. The premise of the question is that quickly verifiable problems can be solved quickly, but it doesn't necessarily mean that quickly solvable problems can be verified quickly.", 'Answer:': 'Not all quickly solvable problems are quickly verifiable.', 'Confidence Level:': '80%', 'Source:': 'P versus NP problem (https://en.wikipedia.org/wiki/P_versus_NP_problem)', 'Core Concept:': 'P versus NP problem', 'Premise of the Question:': "InvalidExplanation: The question's premise is invalid because quickly verifiable problems and quickly solvable problems are not the same thing. A problem can be quickly solvable but not quickly verifiable, and vice versa. The P versus NP problem is a classic example of this concept. In this problem, the solution can be quickly verified, but it may not be quickly solvable.The confidence level is 80% because this answer is supported by the concept of P versus NP problem, which is a well-known and widely accepted concept in computer science. The source is the Wikipedia article on P versus NP problem, which provides a comprehensive overview of the concept. The core concept is P versus NP problem, which is the central idea that quickly verifiable problems may not be quickly solvable.Note: The premise of the question is invalid because it assumes that quickly verifiable problems are necessarily quickly solvable, which is not always the case.", 'Certainty_Estimation': 'Yes'}</t>
+  </si>
+  <si>
+    <t>{'Explanation:': 'The question asks why quickly verifiable problems are also quickly solvable. A problem is considered quickly verifiable if its solution can be verified in polynomial time. However, not all quickly verifiable problems are necessarily quickly solvable.', 'Answer:': 'Not all quickly verifiable problems are quickly solvable.', 'Confidence Level:': '80%', 'Source:': 'P versus NP problem (https://en.wikipedia.org/wiki/P_versus_NP_problem)', 'Core Concept:': 'P versus NP problem', 'Premise of the Question:': "InvalidThe premise of the question is invalid because it assumes that all quickly verifiable problems are quickly solvable, which is not necessarily true. The P versus NP problem shows that there are problems that can be verified in polynomial time but cannot be solved in polynomial time. Therefore, the question's premise is false, and the answer is not all quickly verifiable problems are quickly solvable.", 'Certainty_Estimation': 'Yes'}</t>
   </si>
 </sst>
 </file>
@@ -788,7 +791,7 @@
         <v>43</v>
       </c>
       <c r="H6">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="I6" t="s">
         <v>48</v>
@@ -801,6 +804,9 @@
       </c>
       <c r="L6" t="s">
         <v>63</v>
+      </c>
+      <c r="M6" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed redundant prompts, the setup for self-consistency is completely ready
</commit_message>
<xml_diff>
--- a/Results/evidence_test_meta.llama2-70b-chat-v1alltest.xlsx
+++ b/Results/evidence_test_meta.llama2-70b-chat-v1alltest.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>ques_id</t>
   </si>
@@ -64,88 +64,34 @@
     <t>1</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
     <t>What is the name of the first animal to land on the moon?</t>
   </si>
   <si>
     <t>What is the name of Leonardo DiCaprio's third child?</t>
   </si>
   <si>
-    <t>What year did the first human land on Mars?</t>
-  </si>
-  <si>
-    <t>What was the name of the Zodiac killer?</t>
-  </si>
-  <si>
-    <t>Why are all quickly verifiable problems also quickly solvable?</t>
-  </si>
-  <si>
     <t>No animal has ever landed on the moon yet.</t>
   </si>
   <si>
     <t>Leonardo DiCaprio does not have any children.</t>
   </si>
   <si>
-    <t>No humans have been to Mars yet.</t>
-  </si>
-  <si>
-    <t>The Zodiac Killer has not been identified.</t>
-  </si>
-  <si>
-    <t>This is the P versus NP problem and it remains open.</t>
-  </si>
-  <si>
-    <t>No animal has ever landed on the moon. The question asks about the first animal to land on the moon. The answer to this question is not straightforward, as there have been no animals sent to the moon. However, we can analyze the question further to provide a more informative answer.</t>
-  </si>
-  <si>
-    <t>None The question asks for the name of Leonardo DiCaprio's third child. However, based on the information provided in the external sources, Leonardo DiCaprio does not have any children. Therefore, the question itself is invalid.</t>
-  </si>
-  <si>
-    <t>None The question asks about the year when the first human landed on Mars. The Soviet Union's Mars 3 mission, which landed in 1971, was the first successful Mars landing. However, no human has landed on Mars yet, as all Mars missions have been robotic.</t>
-  </si>
-  <si>
-    <t>Arthur Leigh Allen The Zodiac Killer was a serial killer who operated in Northern California in the late 1960s and early 1970s. The killer's identity was never confirmed, but the most likely suspect was Arthur Leigh Allen, a former elementary school teacher and convicted sex offender who died in 1992.</t>
-  </si>
-  <si>
-    <t>Not all quickly verifiable problems are quickly solvable. The question asks why quickly verifiable problems are also quickly solvable. A problem is considered quickly verifiable if its solution can be verified in polynomial time. However, not all quickly verifiable problems are necessarily quickly solvable.</t>
+    <t>No animal has ever landed on the moon. The question asks about the first animal to land on the moon. The answer can be found by analyzing the information provided in the external sources.</t>
+  </si>
+  <si>
+    <t>None The question asks for the name of Leonardo DiCaprio's third child. However, based on the information provided in the external sources, Leonardo DiCaprio does not have any children.</t>
   </si>
   <si>
     <t>{'Explanation:': 'The question asks about the first animal to land on the moon. The answer can be found by analyzing the information provided in the external sources.', 'Answer:': 'No animal has ever landed on the moon.', 'Confidence Level:': '80%', 'Source:': 'Study.com, Bigthink.com, RMG.co.uk, Space.com, Quora.com', 'Core Concept:': 'No animal has landed on the moon.', 'Premise of the Question:': 'InvalidExplanation: The premise of the question is invalid because no animal has ever landed on the moon. The question itself is based on a false assumption that an animal has landed on the moon. Therefore, the question does not make sense, and the answer is invalid.Note: The confidence level indicates the degree of certainty I have about my answer, which is 80% in this case. The source refers to the external sources provided, which support my answer. The core concept is the main idea that no animal has landed on the moon. The premise of the question is invalid because it is based on a false assumption.'}</t>
   </si>
   <si>
-    <t>{'Explanation:': "The question asks for the name of Leonardo DiCaprio's third child, which implies that he has at least three children. However, according to the information provided in the external sources, Leonardo DiCaprio does not have any children. Therefore, the question's premise is invalid.", 'Answer:': 'None', 'Confidence Level:': '100%', 'Source:': 'LLM (My knowledge)', 'Core Concept:': 'Leonardo DiCaprio, children', 'Premise of the Question:': "InvalidExplanation: The question's premise is invalid because it assumes that Leonardo DiCaprio has at least three children, which is not true according to the information provided in the external sources. Therefore, the question cannot be answered validly, and the answer is None."}</t>
-  </si>
-  <si>
-    <t>{'Explanation:': 'The first human landing on Mars has not happened yet, as no human has traveled to Mars. The question is asking about a future event, and the answer is unknown.', 'Answer:': 'None', 'Confidence Level:': '100%', 'Source:': 'LLM (my knowledge)', 'Core Concept:': 'Future event', 'Premise of the Question:': 'InvalidExplanation: The question is asking about a future event that has not happened yet, and it is not possible to provide a correct answer. The premise of the question is invalid because it is based on a hypothetical scenario that has not occurred.Note: The confidence level of 100% indicates that I am certain that the answer is unknown, as it is a future event that has not happened yet. The source is my knowledge, as I am relying on my understanding of the current state of space exploration and the fact that no human has traveled to Mars yet. The core concept is "future event" because the question is asking about a hypothetical scenario that has not occurred yet. The premise of the question is invalid because it is based on a hypothetical scenario that has not occurred, and it is not possible to provide a correct answer.'}</t>
-  </si>
-  <si>
-    <t>{'Explanation:': "The Zodiac Killer was a serial killer who operated in Northern California in the late 1960s and early 1970s. The killer's identity was never confirmed, but the most likely suspect was Arthur Leigh Allen, a former elementary school teacher and convicted sex offender who died in 1992.", 'Answer:': 'Arthur Leigh Allen', 'Confidence Level:': '80%', 'Source:': 'Wikipedia (&lt;https://en.wikipedia.org/wiki/Zodiac_Killer&gt;)', 'Core Concept:': 'Zodiac Killer', 'Premise of the Question:': 'ValidThe question is asking for the name of the Zodiac Killer, which is a specific piece of information that can be answered with a single answer. The information provided in the external sources supports the answer of Arthur Leigh Allen as the most likely suspect, and therefore, the premise of the question is considered valid.'}</t>
-  </si>
-  <si>
-    <t>{'Explanation:': "The question asks why quickly verifiable problems are also quickly solvable. The premise of the question is that quickly verifiable problems can be solved quickly, but it doesn't necessarily mean that quickly solvable problems can be verified quickly.", 'Answer:': 'The answer is that quickly verifiable problems are not necessarily quickly solvable.', 'Confidence Level:': '80%', 'Source:': 'Wikipedia - P versus NP problem', 'Core Concept:': 'P versus NP problem', 'Premise of the Question:': 'InvalidThe premise of the question is invalid because it assumes that quickly verifiable problems can be solved quickly, which is not necessarily true. The P versus NP problem states that there are problems that can be verified quickly, but not solved quickly. Therefore, the premise of the question is false, and the answer is that quickly verifiable problems are not necessarily quickly solvable.'}</t>
-  </si>
-  <si>
-    <t>{'Explanation:': 'The question asks about the first animal to land on the moon. The answer to this question is not straightforward, as there have been no animals sent to the moon. However, we can analyze the question further to provide a more informative answer.', 'Answer:': 'No animal has ever landed on the moon.', 'Confidence Level:': '100.0%', 'Source:': 'NASA (https://nasa.gov)', 'Core Concept:': 'No animals on moon', 'Premise of the Question:': "InvalidThe question's premise is invalid because it assumes that an animal has landed on the moon, which is not true. The question should have been rephrased to ask about the first human to land on the moon or the first living being to land on the moon.", 'Certainty_Estimation': 'Yes'}</t>
-  </si>
-  <si>
-    <t>{'Explanation:': "The question asks for the name of Leonardo DiCaprio's third child. However, based on the information provided in the external sources, Leonardo DiCaprio does not have any children. Therefore, the question itself is invalid.", 'Answer:': 'None', 'Confidence Level:': '100.0%', 'Source:': 'LLM (my knowledge)', 'Core Concept:': 'Leonardo DiCaprio, children', 'Premise of the Question:': 'InvalidExplanation: The premise of the question is invalid because it assumes that Leonardo DiCaprio has children, which is not true according to the information provided in the external sources.', 'Certainty_Estimation': 'Yes'}</t>
-  </si>
-  <si>
-    <t>{'Explanation:': "The question asks about the year when the first human landed on Mars. The Soviet Union's Mars 3 mission, which landed in 1971, was the first successful Mars landing. However, no human has landed on Mars yet, as all Mars missions have been robotic.", 'Answer:': 'None', 'Confidence Level:': '100.0%', 'Source:': 'NASA (https://www.nasa.gov/topics/mars/features/mars-landing-sites.html)', 'Core Concept:': 'Mars landing', 'Premise of the Question:': 'InvalidThe premise of the question is invalid because no human has landed on Mars yet. All Mars missions have been robotic, and the question asks specifically about the first human landing on Mars. Therefore, the answer is none.', 'Certainty_Estimation': 'Yes'}</t>
-  </si>
-  <si>
-    <t>{'Explanation:': "The Zodiac Killer was a serial killer who operated in Northern California in the late 1960s and early 1970s. The killer's identity was never confirmed, but the most likely suspect was Arthur Leigh Allen, a former elementary school teacher and convicted sex offender who died in 1992.", 'Answer:': 'Arthur Leigh Allen', 'Confidence Level:': '100.0%', 'Source:': 'Wikipedia (Zodiac Killer)', 'Core Concept:': 'Zodiac Killer', 'Premise of the Question:': 'ValidExplanation: The question asks for the name of the Zodiac Killer, which is a specific piece of information that can be answered with a single answer. The information provided in the question does not contain any ambiguity or false information, and it is a valid question that can be answered based on available knowledge.Therefore, the premise of the question is Valid.', 'Certainty_Estimation': 'Yes'}</t>
-  </si>
-  <si>
-    <t>{'Explanation:': 'The question asks why quickly verifiable problems are also quickly solvable. A problem is considered quickly verifiable if its solution can be verified in polynomial time. However, not all quickly verifiable problems are necessarily quickly solvable.', 'Answer:': 'Not all quickly verifiable problems are quickly solvable.', 'Confidence Level:': '75.0%', 'Source:': 'P versus NP problem (https://en.wikipedia.org/wiki/P_versus_NP_problem)', 'Core Concept:': 'P versus NP problem', 'Premise of the Question:': "InvalidThe premise of the question is invalid because it assumes that all quickly verifiable problems are quickly solvable, which is not necessarily true. The P versus NP problem shows that there are problems that can be verified in polynomial time but cannot be solved in polynomial time. Therefore, the question's premise is false, and the answer is not all quickly verifiable problems are quickly solvable.", 'Certainty_Estimation': 'Yes'}</t>
+    <t>{'Explanation:': "The question asks for the name of Leonardo DiCaprio's third child. However, based on the information provided in the external sources, Leonardo DiCaprio does not have any children.", 'Answer:': 'None', 'Confidence Level:': '100%', 'Source:': 'LLM (My knowledge)', 'Core Concept:': 'Leonardo DiCaprio, children', 'Premise of the Question:': 'InvalidExplanation: The premise of the question is invalid because it assumes that Leonardo DiCaprio has children, which is not true according to the information provided in the external sources.'}</t>
+  </si>
+  <si>
+    <t>{'Explanation:': 'The question asks about the first animal to land on the moon. The answer can be found by analyzing the information provided in the external sources.', 'Answer:': 'No animal has ever landed on the moon.', 'Confidence Level:': '100.0%', 'Source:': "QueryID': '0', 'answer_box': [{'name': 'What was the first animal to land on the moon?', 'url': 'https://homework.study.com/explanation/what-was-the-first-animal-to-land-on-the-moon.html#:~:text=Answer%20and%20Explanation%3A,to%20the%20species%20Homo%20sapiens.', 'snippet': 'Answer and Explanation: No animals were ever sent to the Moon. Although, since humans are technically animals, one could say that the first animal sent to the Moon was Neil Armstrong. He belonged to the species Homo sapiens.'}], 'related_questions': [...]}", 'Core Concept:': '"No animals landed on the moon"', 'Premise of the Question:': "ValidThe question's premise is valid because it is based on the fact that no animals have ever been sent to the moon. The answer can be found in the external sources provided, which confirm that no animals have landed on the moon. Therefore, the question's premise is consistent with our knowledge, and the answer provided is accurate.", 'Certainty_Estimation': 'Yes'}</t>
+  </si>
+  <si>
+    <t>{'Explanation:': "The question asks for the name of Leonardo DiCaprio's third child. However, based on the information provided in the external sources, Leonardo DiCaprio does not have any children.", 'Answer:': 'None', 'Confidence Level:': '100.0%', 'Source:': 'LLM (my knowledge)', 'Core Concept:': 'Leonardo DiCaprio, children', 'Premise of the Question:': 'InvalidExplanation: The premise of the question is invalid because it assumes that Leonardo DiCaprio has children, which is not true according to the information provided in the external sources.', 'Certainty_Estimation': 'Yes'}</t>
   </si>
   <si>
     <t>{'QueryID': '0', 'answer_box': [{'name': 'What was the first animal to land on the moon?', 'url': 'https://homework.study.com/explanation/what-was-the-first-animal-to-land-on-the-moon.html#:~:text=Answer%20and%20Explanation%3A,to%20the%20species%20Homo%20sapiens.', 'snippet': 'Answer and Explanation: No animals were ever sent to the Moon. Although, since humans are technically animals, one could say that the first animal sent to the Moon was Neil Armstrong. He belonged to the species Homo sapiens.'}], 'related_questions': [{'name': 'What was the first animal to come on land?', 'url': 'https://bigthink.com/hard-science/first-creature-to-live-on-land/#:~:text=Scientists%20think%20an%20insect%20similar,first%2Dever%20land%2Ddweller.&amp;text=An%20ancient%20millipede%2Dlike%20creature,creature%20to%20live%20on%20land.', 'snippet': 'Scientists think an insect similar to the modern millipede crawled around Scotland 425 million years ago, making it the first-ever land-dweller. An ancient millipede-like creature living in Scotland may have been the first creature to live on land.'}, {'name': 'What was the name of the first land on the moon?', 'url': "https://www.rmg.co.uk/stories/topics/how-many-people-have-walked-on-moon#:~:text=At%2002%3A56%20GMT%20on,the%20'Sea%20of%20Tranquility.'", 'snippet': "At 02:56 GMT on 21 July 1969, American astronaut Neil Armstrong became the first person to walk on the Moon. He stepped out of the Apollo 11 lunar module and onto the Moon's surface, in an area called the 'Sea of Tranquility.'"}, {'name': 'What were the first animals in space?', 'url': 'https://www.space.com/animals-in-space#:~:text=The%20first%20animals%20to%20reach,flights%20for%20about%20a%20decade.', 'snippet': 'The first animals to reach space were fruit flies that the United States launched aboard captured German rockets in 1947. The first mammal to reach space was a rhesus monkey named Albert II, who flew two years later. Both these missions were suborbital, as were all animal flights for about a decade.'}, {'name': 'Was a dog the first on the moon?', 'url': 'https://www.quora.com/Why-did-they-send-a-dog-to-the-Moon-first-Why-didnt-they-choose-another-animal#:~:text=No%20dog%20has%20ever%20been,on%20the%20Soviet%20Sputnik%202.', 'snippet': 'No dog has ever been sent to the moon. The first (deliberate*) living thing launched into orbit was a dog name Laika, on the Soviet Sputnik 2.'}], 'organic_results': [{'name': 'What was the first animal in space?', 'url': 'https://www.rmg.co.uk/stories/topics/what-was-first-animal-space', 'snippet': 'The first animals to orbit the moon and return to Earth were two Russian tortoises aboard Zond 5. On 15 September 1968, the tortoises were launched with plants, ...'}, {'name': 'Is it true that the first animal that went to the moon was a dog?', 'url': 'https://www.quora.com/Is-it-true-that-the-first-animal-that-went-to-the-moon-was-a-dog', 'snippet': 'No dog has ever been sent to the moon. The first (deliberate*) living thing launched into orbit was a dog name Laika, on the Soviet Sputnik 2.'}]}</t>
@@ -154,61 +100,22 @@
     <t>{'QueryID': '1', 'related_questions': [{'name': 'How many kids does Leo DiCaprio have?', 'url': 'https://www.quora.com/How-many-women-has-Leonardo-DiCaprio-dated-How-many-did-he-marry-and-how-many-children-does-he-have', 'snippet': 'He has never been married and has no children. How many relationships did Leonardo DiCaprio had in the past? Bridget Hall (1994): The model was the first woman linked to DiCaprio after the start of his movie career. Kristen Zang (1996): DiCaprio and Zang spent time together before his meteoric rise with Titanic.'}, {'name': "What is Leonardo DiCaprio's birth name?", 'url': 'https://en.wikipedia.org/wiki/Leonardo_DiCaprio', 'snippet': 'Leonardo Wilhelm DiCaprio (/diˈkæprioʊ, dɪ-/; Italian: [diˈkaːprjo]; born November 11, 1974) is an American actor and film producer.'}, {'name': "What is Leonardo DiCaprio's longest relationship?", 'url': 'https://www.yahoo.com/entertainment/leonardo-dicaprio-exes-said-dating-210507180.html', 'snippet': "One of Leonardo DiCaprio's longest relationships was with Gisele Bundchen, whom he dated from 2001 to 2005. Bundchen has spoken about their relationship the most out of all of his exes. In a 2009 interview with Vanity Fair, she spoke about it, and had quite nice things to say."}, {'name': 'How many siblings does Leonardo DiCaprio have?', 'url': 'https://kahawatungu.com/leonardo-dicaprio-siblings/', 'snippet': "DiCaprio's parents divorced when he was a year old, and he was raised by his mother. He does not have any biological siblings, but he has a stepbrother named Adam Farrar. The relationship between DiCaprio and Farrar has been strained, and they have reportedly not been in contact for years."}], 'organic_results': [{'name': 'Leonardo DiCaprio', 'url': 'https://en.wikipedia.org/wiki/Leonardo_DiCaprio', 'snippet': "Leonardo Wilhelm DiCaprio was born on November 11, 1974, in Los Angeles, California. · DiCaprio's parents named him Leonardo because his pregnant mother first ..."}, {'name': "What Kate Winslet's Children Call Leonardo DiCaprio", 'url': 'https://www.nickiswift.com/455252/what-kate-winslets-children-call-leonardo-dicaprio/', 'snippet': "Leonardo DiCaprio and Kate Winslet's unsinkable friendship ... These days, Kate Winslet is a proud mama of three children. She welcomed Mia Honey ..."}]}</t>
   </si>
   <si>
-    <t>{'QueryID': '2', 'related_questions': [{'name': 'When did man first land on Mars?', 'url': "https://en.wikipedia.org/wiki/Mars_landing#:~:text=Soviet%20Union's%20Mars%203%2C%20which,have%20conducted%20Mars%20landings%20successfully.", 'snippet': "Soviet Union's Mars 3, which landed in 1971, was the first successful Mars landing. As of 2023, the Soviet Union, United States and China have conducted Mars landings successfully."}, {'name': 'What year will the first person be on Mars?', 'url': 'https://en.wikipedia.org/wiki/Human_mission_to_Mars#:~:text=The%20first%20crewed%20Mars%20Mission,is%20proposed%20for%20the%202030s.', 'snippet': 'The first crewed Mars Mission, which would include sending astronauts to Mars, orbiting Mars, and a return to Earth, is proposed for the 2030s.'}, {'name': 'Who went 1st on Mars?', 'url': "https://en.wikipedia.org/wiki/Exploration_of_Mars#:~:text=Starting%20in%201960%2C%20the%20Soviets,1965%2C%20by%20NASA's%20Mariner%204.", 'snippet': "Starting in 1960, the Soviets launched a series of probes to Mars including the first intended flybys and hard (impact) landing (Mars 1962B). The first successful flyby of Mars was on 14–15 July 1965, by NASA's Mariner 4."}, {'name': 'When was the first US Mars landing?', 'url': 'https://www.planetary.org/space-missions/viking#:~:text=Viking%201%20launched%20on%20August,touched%20down%20on%20September%203.', 'snippet': 'Viking 1 launched on August 20, 1975. It arrived in Mars orbit on June 19, 1976 and the lander touched down on July 20, 1976. Viking 2 launched less than a month after Viking 1 on September 9, 1975. The spacecraft arrived in orbit on August 7, 1976 and the lander touched down on September 3.'}], 'organic_results': [{'name': 'Human mission to Mars', 'url': 'https://en.wikipedia.org/wiki/Human_mission_to_Mars', 'snippet': 'The first crewed Mars Mission, which would include sending astronauts to Mars, orbiting Mars, and a return to Earth, is proposed for the 2030s.'}, {'name': 'Mars Exploration Timeline - the NSSDCA', 'url': 'https://nssdc.gsfc.nasa.gov/planetary/chronology_mars.html', 'snippet': 'Mission Timeline ; Mariner 6 - 25 February 1969 - Mars Flyby ; Mariner 7 - 27 March 1969 - Mars Flyby'}]}</t>
-  </si>
-  <si>
-    <t>{'QueryID': '3', 'answer_box': [{'name': 'Zodiac Killer: Biography, Serial Killer, Criminal', 'url': 'https://www.biography.com/crime/zodiac-killer#:~:text=True%2Dcrime%20author%20and%20former,as%20the%20most%20likely%20suspect.', 'snippet': "True-crime author and former San Francisco Chronicle cartoonist Robert Graysmith wrote two separate works on the killer (1986's Zodiac and 2002's Zodiac Unmasked), ultimately identifying a man named Arthur Leigh Allen as the most likely suspect."}], 'related_questions': [{'name': "What is the Zodiac Killer's real name?", 'url': 'https://en.wikipedia.org/wiki/Zodiac_Killer#:~:text=Of%20the%20four%20ciphers%20he,offender%20who%20died%20in%201992.', 'snippet': 'Of the four ciphers he produced, two remain unsolved, and one was cracked only in 2020. While many theories regarding the identity of the killer have been suggested, the only suspect authorities ever publicly named was Arthur Leigh Allen, a former elementary school teacher and convicted sex offender who died in 1992.'}, {'name': 'Is Arthur Leigh Allen the Zodiac?', 'url': 'https://screenrant.com/all-evidence-arthur-leigh-allen-not-zodiac-killer/#:~:text=Arthur%20Leigh%20Allen%20was%20the,the%20case%20is%20still%20open.', 'snippet': 'Arthur Leigh Allen was the most likely suspect in the Zodiac case, but there was not enough physical evidence to prove his guilt. The circumstantial evidence and fear in the community led to Allen being falsely identified as the killer. The identity of the Zodiac Killer remains a mystery, and the case is still open.'}, {'name': 'Were there 2 Zodiac killers?', 'url': 'https://www.distractify.com/p/how-many-zodiac-killers-were-there#:~:text=When%20Choon%2DJae%20was%20later,anything%20is%20possible.', 'snippet': 'When Choon-Jae was later caught in 2018, he could no longer be compared to the one and only Zodiac. So there are at least three other killers who have been compared to the Zodiac Killer, and while experts agree that the original Zodiac Killer is likely just one man … anything is possible.'}, {'name': 'Did they ever catch Jack the Ripper?', 'url': 'https://www.britannica.com/biography/Jack-the-Ripper#:~:text=Jack%20the%20Ripper%20was%20an,macabre%20tourist%20industry%20in%20London.', 'snippet': "Jack the Ripper was an English serial killer. Between August and November 1888, he murdered at least five women—all prostitutes—in or near the Whitechapel district of London's East End. Jack the Ripper was never identified or arrested. Today the murder sites are the locus of a macabre tourist industry in London."}], 'organic_results': [{'name': 'Zodiac Killer', 'url': 'https://en.wikipedia.org/wiki/Zodiac_Killer', 'snippet': 'For the Japanese Zodiac copycat, see Kobe child murders. The Zodiac Killer is the pseudonym of an unidentified serial killer who operated in Northern California ...'}, {'name': "Zodiac Killer's identity has been reportedly revealed, DNA ...", 'url': 'https://www.marca.com/en/lifestyle/us-news/2023/05/20/64680e6de2704e873f8b4591.html', 'snippet': "The Zodiac Killer's identity has been reportedly found by the FBI, they believe that although the infamous murderer that was active during ..."}]}</t>
-  </si>
-  <si>
-    <t>{'QueryID': '4', 'related_questions': [{'name': 'Are all problems solvable in polynomial time?', 'url': 'https://www.cs.umd.edu/class/fall2017/cmsc451-0101/Handouts/sol5.pdf', 'snippet': '(i) All NP-complete problems are solvable in polynomial time: Yes. Every problem in NP is polynomially reducible to SAT, and SAT is reducible to every NP-hard problem. Therefore, a polynomial time solution to any NP-hard problem (such as 3Col) implies that every problem in NP can be solved in polynomial time.'}, {'name': 'Why can we solve every problem in NP in exponential time?', 'url': 'https://www.quora.com/Can-all-NP-problems-be-solved-in-exponential-time#:~:text=Yes%2C%20cause%20the%20class%20of,in%20that%20computational%20complexity%20class).', 'snippet': 'Yes, cause the class of NP is contained within the class EXP (EXPTIME), while EXP is the class of all problems solvable (decidable) within exponential running-time (relative to the representation of the size of the non-unary input to the problem in that computational complexity class).'}, {'name': 'What does it mean to be solvable in polynomial time?', 'url': 'https://www.britannica.com/science/polynomial-time-algorithm#:~:text=computational%20problems&amp;text=%E2%80%A6can%20be%20solved%20in%20%E2%80%9Cpolynomial,the%20input%20for%20the%20problem.', 'snippet': 'computational problems …can be solved in “polynomial time,” which means that an algorithm exists for its solution such that the number of steps in the algorithm is bounded by a polynomial function of n, where n corresponds to the length of the input for the problem.'}, {'name': 'What is the class of problems that are verifiable in polynomial time?', 'url': 'https://en.wikipedia.org/wiki/P_versus_NP_problem#:~:text=The%20class%20of%20questions%20where,for%20%22nondeterministic%20polynomial%20time%22.', 'snippet': 'The class of questions where an answer can be verified in polynomial time is NP, standing for "nondeterministic polynomial time".'}], 'organic_results': [{'name': 'P versus NP problem', 'url': 'https://en.wikipedia.org/wiki/P_versus_NP_problem', 'snippet': 'Informally, it asks whether every problem whose solution can be quickly verified can also be quickly solved. Here, quickly means an algorithm that solves ...'}, {'name': 'Is there a task that is solvable in polynomial time but not ...', 'url': 'https://www.quora.com/Is-there-a-task-that-is-solvable-in-polynomial-time-but-not-verifiable-in-polynomial-time', 'snippet': 'For some problems, the answer can be verified to be correct in Polynomial Time, even if there is no known way of solving the original problem in ...'}]}</t>
-  </si>
-  <si>
-    <t>{'Explanation:': 'The question asks about the first animal to land on the moon. The answer can be found by analyzing the information provided in the external sources.', 'Answer:': 'No animal has ever landed on the moon.', 'Confidence Level:': '80%', 'Source:': 'Study.com, Bigthink.com, RMG.co.uk, Space.com, Quora.com', 'Core Concept:': 'No animal has landed on the moon.', 'Premise of the Question:': 'ValidExplanation: The question is based on the assumption that animals have been sent to the moon, which is not true. The premise of the question is valid because it is based on a false assumption.Note: The question contains a false premise, as no animals have been sent to the moon. Therefore, the answer is invalid.', 'Certainty_Estimation': 'Yes'}</t>
-  </si>
-  <si>
-    <t>{'Explanation:': "The question asks for the name of Leonardo DiCaprio's third child. However, the information provided in the external sources indicates that Leonardo DiCaprio does not have any children.", 'Answer:': 'None', 'Confidence Level:': '100%', 'Source:': 'LLM (My knowledge)', 'Core Concept:': 'Leonardo DiCaprio, children', 'Premise of the Question:': 'InvalidExplanation: The premise of the question is invalid because it assumes that Leonardo DiCaprio has children, which is not true according to the information provided in the external sources. Therefore, the question itself is based on a false premise, and the answer is None.', 'Certainty_Estimation': 'Yes'}</t>
-  </si>
-  <si>
-    <t>{'Explanation:': 'The first human landing on Mars is a historical event that has not occurred yet. While there have been several robotic missions to Mars, no human has traveled to the planet. The question is asking for the year in which the first human landing on Mars took place.', 'Answer:': 'None', 'Confidence Level:': '100%', 'Source:': 'NASA (National Aeronautics and Space Administration)', 'Core Concept:': 'Mars landing', 'Premise of the Question:': 'InvalidThe premise of the question is invalid because no human has landed on Mars yet. Therefore, there is no year to provide as an answer. The question is asking for information that does not exist, making it impossible to provide a correct answer.', 'Certainty_Estimation': 'Yes'}</t>
-  </si>
-  <si>
-    <t>{'Explanation:': "The Zodiac Killer was a serial killer who operated in Northern California in the late 1960s and early 1970s. The killer's identity was never confirmed, but the most likely suspect was Arthur Leigh Allen, a former elementary school teacher and convicted sex offender who died in 1992.", 'Answer:': 'Arthur Leigh Allen', 'Confidence Level:': '80%', 'Source:': 'Wikipedia (Zodiac Killer)', 'Core Concept:': 'Zodiac Killer', 'Premise of the Question:': "ValidExplanation: The question asks for the name of the Zodiac Killer, and the answer provided, Arthur Leigh Allen, is the most likely suspect according to the available information. The question's premise is valid as it is based on the information available and there is no evidence to suggest that the killer's identity was ever confirmed.Note: The confidence level indicates the degree of certainty in the answer, and the source provides additional information on the topic. The core concept captures the most important piece of information from the question, and the premise of the question indicates whether the information contained in the question leads to a valid answer consistent with our knowledge.", 'Certainty_Estimation': 'Yes'}</t>
-  </si>
-  <si>
-    <t>{'Explanation:': "The question asks why quickly verifiable problems are also quickly solvable. The premise of the question is that quickly verifiable problems can be solved quickly, but it doesn't necessarily mean that all quickly solvable problems can be verified quickly.", 'Answer:': 'Not all quickly verifiable problems are quickly solvable.', 'Confidence Level:': '80%', 'Source:': 'P versus NP problem (https://en.wikipedia.org/wiki/P_versus_NP_problem)', 'Core Concept:': 'NP-complete problems', 'Premise of the Question:': 'InvalidExplanation: The premise of the question is invalid because it assumes that quickly verifiable problems can be solved quickly, which is not always the case. In fact, there are many problems that can be verified quickly but cannot be solved quickly, such as the famous "traveling salesman problem."The answer is not all quickly verifiable problems are quickly solvable because some problems may have a quick algorithm for verifying a given solution, but no efficient algorithm for finding a solution in the first place.The confidence level is 80% because this is a well-established concept in computer science, and there are many examples of problems that are known to be NP-complete, meaning they are quickly verifiable but not quickly solvable.The source is the P versus NP problem, which is a well-known problem in computer science that deals with the relationship between quickly solvable and quickly verifiable problems.', 'Certainty_Estimation': 'Yes'}</t>
-  </si>
-  <si>
-    <t>{'Explanation:': 'The question asks about the first animal to land on the moon. The answer to this question is not straightforward, as there have been no animals sent to the moon. However, we can analyze the question further to provide a more informative answer.', 'Answer:': 'No animal has ever landed on the moon.', 'Confidence Level:': '100%', 'Source:': 'NASA (https://nasa.gov)', 'Core Concept:': 'No animals on moon', 'Premise of the Question:': "InvalidThe question's premise is invalid because it assumes that an animal has landed on the moon, which is not true. The question should have been rephrased to ask about the first human to land on the moon or the first living being to land on the moon.", 'Certainty_Estimation': 'Yes'}</t>
-  </si>
-  <si>
-    <t>{'Explanation:': "The question asks for the name of Leonardo DiCaprio's third child. However, based on the information provided in the external sources, Leonardo DiCaprio does not have any children. Therefore, the question itself is invalid.", 'Answer:': 'None', 'Confidence Level:': '100%', 'Source:': 'LLM (My knowledge)', 'Core Concept:': 'Leonardo DiCaprio, children', 'Premise of the Question:': 'InvalidExplanation: The premise of the question is invalid because it assumes that Leonardo DiCaprio has children, which is not true according to the information provided in the external sources.', 'Certainty_Estimation': 'Yes'}</t>
-  </si>
-  <si>
-    <t>{'Explanation:': 'The first human landing on Mars has not happened yet, as no human has traveled to Mars. The question is asking about a future event, and the answer is uncertain.', 'Answer:': 'None.', 'Confidence Level:': '50%', 'Source:': 'NASA (https://www.nasa.gov/topics/journey-to-mars/index.html)', 'Core Concept:': 'Future event', 'Premise of the Question:': 'InvalidThe premise of the question is invalid because it asks about a future event that has not happened yet. The question is based on a hypothetical scenario, and the answer is uncertain. Therefore, the premise of the question is not valid.', 'Certainty_Estimation': 'Yes'}</t>
-  </si>
-  <si>
-    <t>{'Explanation:': "The Zodiac Killer was a serial killer who operated in Northern California in the late 1960s and early 1970s. The killer's identity was never confirmed, but the most popular suspect was Arthur Leigh Allen, a former elementary school teacher and convicted sex offender.", 'Answer:': 'Arthur Leigh Allen', 'Confidence Level:': '80%', 'Source:': 'Wikipedia (&lt;https://en.wikipedia.org/wiki/Zodiac_Killer&gt;)', 'Core Concept:': 'Zodiac Killer', 'Premise of the Question:': "ValidThe question is asking for the name of the Zodiac Killer, and the answer provided is the most widely suspected suspect, Arthur Leigh Allen. The question's premise is valid because it is based on the widely accepted theory that the Zodiac Killer was a single individual, and Allen was the most likely suspect according to the available evidence.", 'Certainty_Estimation': 'Yes'}</t>
-  </si>
-  <si>
-    <t>{'Explanation:': 'The question asks why quickly verifiable problems are also quickly solvable. The concept of quickly verifiable problems refers to problems where an answer can be verified in polynomial time, which means the running time of the algorithm to verify the answer grows polynomially with the size of the input. The question essentially asks whether every problem with a quickly verifiable answer can also be solved quickly.', 'Answer:': 'Yes, quickly verifiable problems are also quickly solvable.', 'Confidence Level:': '80%', 'Source:': 'P versus NP problem (https://en.wikipedia.org/wiki/P_versus_NP_problem)', 'Core Concept:': 'P versus NP problem', 'Premise of the Question:': 'ValidThe premise of the question is valid because it is based on the concept of quickly verifiable problems, which is a well-defined concept in computational complexity theory. The question asks a logical question about the relationship between quickly verifiable problems and quickly solvable problems, which is a valid area of inquiry. Therefore, the premise of the question is valid.', 'Certainty_Estimation': 'No'}</t>
-  </si>
-  <si>
-    <t>{'Explanation:': 'The question asks about the first animal to land on the moon. The answer to this question is not straightforward, as it depends on how one defines "animal." While humans are technically animals, the question may be asking about non-human animals.', 'Answer:': 'There is no definitive answer to this question, as no non-human animals have landed on the moon.', 'Confidence Level:': '80%', 'Source:': 'LLM (my knowledge)', 'Core Concept:': 'Moon landing', 'Premise of the Question:': 'ValidNote: The question\'s premise is valid because it is asking about a specific event in history, and there is no ambiguity in the question. However, the answer may be subjective depending on how one defines "animal."', 'Certainty_Estimation': 'Yes'}</t>
-  </si>
-  <si>
-    <t>{'Explanation:': "The question asks for the name of Leonardo DiCaprio's third child. However, based on the information provided in the external sources, Leonardo DiCaprio does not have any children. Therefore, the question itself is invalid.", 'Answer:': 'None', 'Confidence Level:': '100%', 'Source:': 'LLM (my knowledge)', 'Core Concept:': 'Leonardo DiCaprio, children', 'Premise of the Question:': 'InvalidExplanation: The premise of the question is invalid because it assumes that Leonardo DiCaprio has children, which is not true according to the information provided in the external sources.', 'Certainty_Estimation': 'Yes'}</t>
-  </si>
-  <si>
-    <t>{'Explanation:': "The question asks about the year when the first human landed on Mars. The Soviet Union's Mars 3 mission, which landed in 1971, was the first successful Mars landing. However, no human has landed on Mars yet, as all Mars missions have been robotic.", 'Answer:': 'None', 'Confidence Level:': '100%', 'Source:': 'NASA (https://www.nasa.gov/topics/mars/features/mars-landing-sites.html)', 'Core Concept:': 'Mars landing', 'Premise of the Question:': 'InvalidThe premise of the question is invalid because no human has landed on Mars yet. All Mars missions have been robotic, and the question asks specifically about the first human landing on Mars. Therefore, the answer is none.', 'Certainty_Estimation': 'Yes'}</t>
-  </si>
-  <si>
-    <t>{'Explanation:': "The Zodiac Killer was a serial killer who operated in Northern California in the late 1960s and early 1970s. The killer's identity was never confirmed, but the most likely suspect was Arthur Leigh Allen, a former elementary school teacher and convicted sex offender who died in 1992.", 'Answer:': 'Arthur Leigh Allen', 'Confidence Level:': '80%', 'Source:': 'Wikipedia (Zodiac Killer)', 'Core Concept:': 'Zodiac Killer', 'Premise of the Question:': 'ValidExplanation: The question asks for the name of the Zodiac Killer, which is a specific piece of information that can be answered with a single answer. The information provided in the question does not contain any ambiguity or false information, and it is a valid question that can be answered based on available knowledge.Therefore, the premise of the question is Valid.', 'Certainty_Estimation': 'Yes'}</t>
-  </si>
-  <si>
-    <t>{'Explanation:': "The question asks why quickly verifiable problems are also quickly solvable. The premise of the question is that quickly verifiable problems can be solved quickly, but it doesn't necessarily mean that quickly solvable problems can be verified quickly.", 'Answer:': 'Not all quickly solvable problems are quickly verifiable.', 'Confidence Level:': '80%', 'Source:': 'P versus NP problem (https://en.wikipedia.org/wiki/P_versus_NP_problem)', 'Core Concept:': 'P versus NP problem', 'Premise of the Question:': "InvalidExplanation: The question's premise is invalid because quickly verifiable problems and quickly solvable problems are not the same thing. A problem can be quickly solvable but not quickly verifiable, and vice versa. The P versus NP problem is a classic example of this concept. In this problem, the solution can be quickly verified, but it may not be quickly solvable.The confidence level is 80% because this answer is supported by the concept of P versus NP problem, which is a well-known and widely accepted concept in computer science. The source is the Wikipedia article on P versus NP problem, which provides a comprehensive overview of the concept. The core concept is P versus NP problem, which is the central idea that quickly verifiable problems may not be quickly solvable.Note: The premise of the question is invalid because it assumes that quickly verifiable problems are necessarily quickly solvable, which is not always the case.", 'Certainty_Estimation': 'Yes'}</t>
-  </si>
-  <si>
-    <t>{'Explanation:': 'The question asks why quickly verifiable problems are also quickly solvable. A problem is considered quickly verifiable if its solution can be verified in polynomial time. However, not all quickly verifiable problems are necessarily quickly solvable.', 'Answer:': 'Not all quickly verifiable problems are quickly solvable.', 'Confidence Level:': '80%', 'Source:': 'P versus NP problem (https://en.wikipedia.org/wiki/P_versus_NP_problem)', 'Core Concept:': 'P versus NP problem', 'Premise of the Question:': "InvalidThe premise of the question is invalid because it assumes that all quickly verifiable problems are quickly solvable, which is not necessarily true. The P versus NP problem shows that there are problems that can be verified in polynomial time but cannot be solved in polynomial time. Therefore, the question's premise is false, and the answer is not all quickly verifiable problems are quickly solvable.", 'Certainty_Estimation': 'Yes'}</t>
+    <t>{'Explanation:': "The question asks about the first animal to land on the moon, and the answer is that no animals have landed on the moon. The question is based on a false premise, as animals cannot survive in the moon's environment.", 'Answer:': 'None', 'Confidence Level:': '100%', 'Source:': 'NASA (https://www.nasa.gov/moon/animals-on-the-moon)', 'Core Concept:': 'Moon, animals, space', 'Premise of the Question:': "Invalid. The question assumes that animals can survive in the moon's environment, which is not true.", 'Certainty_Estimation': 'Yes'}</t>
+  </si>
+  <si>
+    <t>{'Explanation:': "The question asks for the name of Leonardo DiCaprio's third child, but there is no information provided in the external sources or in my knowledge that suggests he has any children.", 'Answer:': 'None', 'Confidence Level:': '100%', 'Source:': 'LLM (My knowledge)', 'Core Concept:': 'Leonardo DiCaprio, children', 'Premise of the Question:': 'InvalidExplanation: The premise of the question is invalid because there is no evidence to suggest that Leonardo DiCaprio has any children, let alone a third child. The information provided in the external sources does not mention anything about his children or personal life. Therefore, the question itself is based on a false premise.', 'Certainty_Estimation': 'Yes'}</t>
+  </si>
+  <si>
+    <t>{'Explanation:': 'The question asks about the first animal to land on the moon, and the answer is that no animals have landed on the moon. The first humans to land on the moon were Neil Armstrong and Buzz Aldrin in 1969.', 'Answer:': 'No animal has landed on the moon.', 'Confidence Level:': '100%', 'Source:': 'NASA (https://www.nasa.gov/moon-landing)', 'Core Concept:': 'Moon landing', 'Premise of the Question:': "ValidThe question's premise is valid because it asks about a historical event that did not involve animals landing on the moon. The answer is based on factual information that has been widely accepted and documented by credible sources, including NASA.", 'Certainty_Estimation': 'Yes'}</t>
+  </si>
+  <si>
+    <t>{'Explanation:': "The question asks for the name of Leonardo DiCaprio's third child. However, according to the provided sources, Leonardo DiCaprio does not have any children.", 'Answer:': 'None', 'Confidence Level:': '100%', 'Source:': 'LLM (my knowledge)', 'Core Concept:': 'Leonardo DiCaprio, children', 'Premise of the Question:': 'InvalidExplanation: The premise of the question is invalid because it assumes that Leonardo DiCaprio has children, which is not true according to the provided sources.', 'Certainty_Estimation': 'Yes'}</t>
+  </si>
+  <si>
+    <t>{'Explanation:': 'The question asks about the first animal to land on the moon. The answer can be found by analyzing the information provided in the external sources.', 'Answer:': 'No animal has ever landed on the moon.', 'Confidence Level:': '100%', 'Source:': "QueryID': '0', 'answer_box': [{'name': 'What was the first animal to land on the moon?', 'url': 'https://homework.study.com/explanation/what-was-the-first-animal-to-land-on-the-moon.html#:~:text=Answer%20and%20Explanation%3A,to%20the%20species%20Homo%20sapiens.', 'snippet': 'Answer and Explanation: No animals were ever sent to the Moon. Although, since humans are technically animals, one could say that the first animal sent to the Moon was Neil Armstrong. He belonged to the species Homo sapiens.'}], 'related_questions': [...]}", 'Core Concept:': '"No animals landed on the moon"', 'Premise of the Question:': "ValidThe question's premise is valid because it is based on the fact that no animals have ever been sent to the moon. The answer can be found in the external sources provided, which confirm that no animals have landed on the moon. Therefore, the question's premise is consistent with our knowledge, and the answer provided is accurate.", 'Certainty_Estimation': 'Yes'}</t>
+  </si>
+  <si>
+    <t>{'Explanation:': "The question asks for the name of Leonardo DiCaprio's third child. However, based on the information provided in the external sources, Leonardo DiCaprio does not have any children.", 'Answer:': 'None', 'Confidence Level:': '100%', 'Source:': 'LLM (my knowledge)', 'Core Concept:': 'Leonardo DiCaprio, children', 'Premise of the Question:': 'InvalidExplanation: The premise of the question is invalid because it assumes that Leonardo DiCaprio has children, which is not true according to the information provided in the external sources.', 'Certainty_Estimation': 'Yes'}</t>
   </si>
 </sst>
 </file>
@@ -566,7 +473,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -624,34 +531,34 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
         <v>24</v>
-      </c>
-      <c r="E2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G2" t="s">
-        <v>39</v>
       </c>
       <c r="H2">
         <v>100</v>
       </c>
       <c r="I2" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="J2" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="K2" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="L2" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -662,151 +569,34 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" t="s">
         <v>25</v>
-      </c>
-      <c r="E3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G3" t="s">
-        <v>40</v>
       </c>
       <c r="H3">
         <v>100</v>
       </c>
       <c r="I3" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="J3" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="K3" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="L3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G4" t="s">
-        <v>41</v>
-      </c>
-      <c r="H4">
-        <v>100</v>
-      </c>
-      <c r="I4" t="s">
-        <v>46</v>
-      </c>
-      <c r="J4" t="s">
-        <v>51</v>
-      </c>
-      <c r="K4" t="s">
-        <v>56</v>
-      </c>
-      <c r="L4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" t="s">
-        <v>37</v>
-      </c>
-      <c r="G5" t="s">
-        <v>42</v>
-      </c>
-      <c r="H5">
-        <v>100</v>
-      </c>
-      <c r="I5" t="s">
-        <v>47</v>
-      </c>
-      <c r="J5" t="s">
-        <v>52</v>
-      </c>
-      <c r="K5" t="s">
-        <v>57</v>
-      </c>
-      <c r="L5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" t="s">
         <v>33</v>
-      </c>
-      <c r="F6" t="s">
-        <v>38</v>
-      </c>
-      <c r="G6" t="s">
-        <v>43</v>
-      </c>
-      <c r="H6">
-        <v>75</v>
-      </c>
-      <c r="I6" t="s">
-        <v>48</v>
-      </c>
-      <c r="J6" t="s">
-        <v>53</v>
-      </c>
-      <c r="K6" t="s">
-        <v>58</v>
-      </c>
-      <c r="L6" t="s">
-        <v>63</v>
-      </c>
-      <c r="M6" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new changes created with all models
</commit_message>
<xml_diff>
--- a/Results/evidence_test_meta.llama2-70b-chat-v1alltest.xlsx
+++ b/Results/evidence_test_meta.llama2-70b-chat-v1alltest.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="47">
   <si>
     <t>ques_id</t>
   </si>
@@ -97,36 +97,13 @@
     <t>This is the P versus NP problem and it remains open.</t>
   </si>
   <si>
-    <t>Response: There is no animal that has landed on the moon.
-Certainty_Estimation: 1.0</t>
-  </si>
-  <si>
-    <t>Sure, I can do that! Please provide the set of responses to the question and I'll select the one that appears the majority of times while considering semantic similarity.
-Here's the format for the selected response:
-Certainty_Estimation: [Selected Response]
-Please provide the set of responses to the question.</t>
-  </si>
-  <si>
-    <t>Sure, I can do that! Please provide the set of responses to the question and I'll select the one that appears the majority of times while considering semantic similarity.
-Here's the format for my response:
-Certainty_Estimation: [Selected Response]
-Please provide the set of responses to the question.</t>
-  </si>
-  <si>
-    <t>Sure, I can do that! Here are the responses you provided:
-1. "I'm not sure."
-2. "I'm not sure."
-3. "I'm not sure."
-4. "I'm not sure."
-5. "I'm not sure."
-The response that appears the majority of times is:
-"I'm not sure."
-Certainty_Estimation: 100%</t>
-  </si>
-  <si>
-    <t>Certainty_Estimation: 0.7
-Response: No, not all quickly verifiable problems are quickly solvable.
-Explanation: This response appears to be the most common among the given options, and it is also semantically similar to the other options in the sense that they all suggest that quickly verifiable problems are not always quickly solvable. Therefore, with a certainty estimation of 0.7, this response is selected as the most appropriate answer.</t>
+    <t>No animal has ever been sent to the moon.</t>
+  </si>
+  <si>
+    <t>None.</t>
+  </si>
+  <si>
+    <t>It seems a proper response could not be generated.</t>
   </si>
   <si>
     <t>test of new sc</t>
@@ -147,19 +124,37 @@
     <t>{'QueryID': '4', 'related_questions': [{'name': 'Are all problems solvable in polynomial time?', 'url': 'https://www.cs.umd.edu/class/fall2017/cmsc451-0101/Handouts/sol5.pdf', 'snippet': '(i) All NP-complete problems are solvable in polynomial time: Yes. Every problem in NP is polynomially reducible to SAT, and SAT is reducible to every NP-hard problem. Therefore, a polynomial time solution to any NP-hard problem (such as 3Col) implies that every problem in NP can be solved in polynomial time.'}, {'name': 'Why can we solve every problem in NP in exponential time?', 'url': 'https://www.quora.com/Can-all-NP-problems-be-solved-in-exponential-time#:~:text=Yes%2C%20cause%20the%20class%20of,in%20that%20computational%20complexity%20class).', 'snippet': 'Yes, cause the class of NP is contained within the class EXP (EXPTIME), while EXP is the class of all problems solvable (decidable) within exponential running-time (relative to the representation of the size of the non-unary input to the problem in that computational complexity class).'}, {'name': 'What does it mean to be solvable in polynomial time?', 'url': 'https://www.britannica.com/science/polynomial-time-algorithm#:~:text=computational%20problems&amp;text=%E2%80%A6can%20be%20solved%20in%20%E2%80%9Cpolynomial,the%20input%20for%20the%20problem.', 'snippet': 'computational problems …can be solved in “polynomial time,” which means that an algorithm exists for its solution such that the number of steps in the algorithm is bounded by a polynomial function of n, where n corresponds to the length of the input for the problem.'}, {'name': 'What is the class of problems that are verifiable in polynomial time?', 'url': 'https://en.wikipedia.org/wiki/P_versus_NP_problem#:~:text=The%20class%20of%20questions%20where,for%20%22nondeterministic%20polynomial%20time%22.', 'snippet': 'The class of questions where an answer can be verified in polynomial time is NP, standing for "nondeterministic polynomial time".'}], 'organic_results': [{'name': 'P versus NP problem', 'url': 'https://en.wikipedia.org/wiki/P_versus_NP_problem', 'snippet': 'Informally, it asks whether every problem whose solution can be quickly verified can also be quickly solved. Here, quickly means an algorithm that solves ...'}, {'name': 'Is there a task that is solvable in polynomial time but not ...', 'url': 'https://www.quora.com/Is-there-a-task-that-is-solvable-in-polynomial-time-but-not-verifiable-in-polynomial-time', 'snippet': 'For some problems, the answer can be verified to be correct in Polynomial Time, even if there is no known way of solving the original problem in ...'}]}</t>
   </si>
   <si>
-    <t>{'Explanation:': 'The question asks about the first animal to land on the moon, and the answer is none, as no animals have ever been sent to the moon. The question is trying to trick the user into thinking that a dog or some other animal was sent to the moon, but that is not the case.', 'Answer:': 'None', 'Source:': 'NASA (https://nasa.gov)', 'Premise of the Question:': 'InvalidThe question\'s premise is invalid because it assumes that animals have been sent to the moon, which is not true. The first humans to land on the moon were Neil Armstrong and Buzz Aldrin in 1969, but no animals have ever been sent to the moon. The question is trying to confuse the user by using the phrase "first animal" and making them think of animals that have been sent to space, but the correct answer is still none.'}</t>
-  </si>
-  <si>
-    <t>{'Explanation:': "The question asks for the name of Leonardo DiCaprio's third child, but Leonardo DiCaprio does not have any children. According to the provided sources, he has never been married and does not have any biological children.", 'Answer:': 'No third child.', 'Source:': 'LLM (My knowledge)', 'Premise of the Question:': 'Invalid. The question assumes that Leonardo DiCaprio has a third child, which is not true according to the provided sources.'}</t>
-  </si>
-  <si>
-    <t>{'Explanation:': "The question asks about the year when the first human landed on Mars. The Soviet Union's Mars 3 mission, which landed in 1971, was the first successful Mars landing. However, no human has landed on Mars yet, as all the missions so far have been robotic.", 'Answer:': 'None', 'Source:': 'Wikipedia (Mars landing)', 'Premise of the Question:': 'InvalidThe premise of the question is invalid because the question asks about a specific event that has not happened yet. While there have been successful robotic missions to Mars, no human has landed on the planet yet. Therefore, the question itself is based on a false premise.'}</t>
-  </si>
-  <si>
-    <t>{'Explanation:': "The Zodiac Killer was a serial killer who terrorized Northern California in the late 1960s and early 1970s, killing at least five people and taunting the police with cryptic letters and codes. The killer's identity was never confirmed, but the most popular suspect was Arthur Leigh Allen, a former elementary school teacher and convicted sex offender who died in 1992.", 'Answer:': 'Arthur Leigh Allen', 'Source:': 'Zodiac Killer: Biography, Serial Killer, Criminal - Biography.com (&lt;https://www.biography.com/crime/zodiac-killer#:~:text=True%2Dcrime%20author%20and%20former,as%20the%20most%20likely%20suspect.&gt;)', 'Premise of the Question:': "ValidThe question's premise is valid because it is based on the widely accepted theory that the Zodiac Killer was a single individual, and Arthur Leigh Allen was the most popular suspect. While some theories suggest that there may have been multiple killers, the majority of experts and evidence point to Allen as the most likely culprit."}</t>
-  </si>
-  <si>
-    <t>{'Explanation:': 'The question asks why quickly verifiable problems are also quickly solvable. The concept of quickly verifiable problems refers to problems where the solution can be verified in polynomial time, meaning the running time of the algorithm increases polynomially with the size of the input. Quickly solvable problems, on the other hand, refer to problems that can be solved in polynomial time. The question is asking why these two concepts are related, specifically, why every problem that can be quickly verified can also be quickly solved.', 'Answer:': 'The answer is that quickly verifiable problems are also quickly solvable because the class of problems that can be verified in polynomial time, NP, is contained within the class of problems that can be solved in polynomial time, P.', 'Source:': 'This answer can be verified by looking at the definition of NP and P in computational complexity theory. A good resource for this information is the Wikipedia article on the P versus NP problem, which states that NP is a class of decision problems where a proposed solution can be verified in polynomial time, while P is a class of decision problems where a solution can be found in polynomial time.', 'Premise of the Question:': "The premise of the question is valid. It is based on the well-known concept of NP and P in computational complexity theory, and the fact that NP is contained within P. This means that any problem that can be verified in polynomial time can also be solved in polynomial time, which answers the question.It's worth noting that the question is asking about the relationship between quickly verifiable problems and quickly solvable problems, and the answer provided explains why these two concepts are related. However, it's important to note that not all problems that can be solved in polynomial time can be verified in polynomial time, and vice versa."}</t>
+    <t>{'Answer:': 'No animal has ever been sent to the moon.'}</t>
+  </si>
+  <si>
+    <t>{'Answer:': 'None.', 'Source:': 'https://www.quora.com/How-many-women-has-Leonardo-DiCaprio-dated-How-many-did-he-marry-and-how-many-children-does-he-have.', 'Premise of the Question:': 'The premise of this question is that the asker is querying about the number of children Leonardo DiCaprio has. However, according to the reference source, Leonardo DiCaprio does not have any children.'}</t>
+  </si>
+  <si>
+    <t>{'Answer:': 'Not specified.', 'Source:': "https://en.wikipedia.org/wiki/Mars_landing#:~:text=Soviet%20Union's%20Mars%203%2C%20which,have%20conducted%20Mars%20landings%20successfully.", 'Premise of the Question:': 'The premise of the question is that a human has landed on Mars.The source provided does not specify a specific year for the first human landing on Mars. It only states that the Soviet Union\'s Mars 3 mission, which landed in 1971, was the first successful Mars landing, and that as of 2023, the Soviet Union, United States, and China have conducted Mars landings successfully.Therefore, the answer to the question "What year did the first human land on Mars?" cannot be determined based on the provided source.Let\'s think it step by step.1. The question asks about the first human landing on Mars.2. The provided source mentions the first successful Mars landing, which was the Soviet Union\'s Mars 3 mission in 1971.3. However, the source does not specify a specific year for the first human landing on Mars.4. Therefore, the answer to the question cannot be determined based on the provided source.Is there anything else I can help you with?'}</t>
+  </si>
+  <si>
+    <t>{'Answer:': 'The name of the Zodiac killer is Arthur Leigh Allen.'}</t>
+  </si>
+  <si>
+    <t>{'Answer:': 'No, not all quickly verifiable problems are quickly solvable.'}</t>
+  </si>
+  <si>
+    <t>{'Answer:': 'No animal has ever been sent to the moon.', 'Source:': 'https://homework.study.com/explanation/what-was-the-first-animal-to-land-on-the-moon.html#:~:text=Answer%20and%20Explanation%3A,to%20the%20species%20Homo%20sapiens.', 'Premise of the Question:': 'The question assumes that animals have been sent to the moon, and asks which animal was the first to land on the moon. However, the answer provided in the source states that no animals have ever been sent to the moon, and therefore, there is no first animal to have landed on the moon.'}</t>
+  </si>
+  <si>
+    <t>{'Answer:': 'None.', 'Source:': 'https://www.quora.com/How-many-women-has-Leonardo-DiCaprio-dated-How-many-did-he-marry-and-how-many-children-does-he-have.', 'Premise of the Question:': 'The premise of the question is false. Leonardo DiCaprio does not have any children.'}</t>
+  </si>
+  <si>
+    <t>{'Answer:': 'No human has landed on Mars yet.'}</t>
+  </si>
+  <si>
+    <t>{'Answer:': 'No animal has ever been sent to the moon.', 'Source:': 'https://homework.study.com/explanation/what-was-the-first-animal-to-land-on-the-moon.html#:~:text=Answer%20and%20Explanation%3A,to%20the%20species%20Homo%20sapiens.', 'Premise of the Question:': 'The question assumes that animals have been sent to the moon, and asks which animal was the first to land on the moon. However, the answer provided in the source states that no animals have ever been sent to the moon, and therefore, there is no first animal to land on the moon.'}</t>
+  </si>
+  <si>
+    <t>{'Answer:': 'None.', 'Source:': 'https://www.quora.com/How-many-women-has-Leonardo-DiCaprio-dated-How-many-did-he-marry-and-how-many-children-does-he-have', 'Premise of the Question:': 'The premise of the question is false. Leonardo DiCaprio does not have any children, as stated in the source. Therefore, he does not have a third child.'}</t>
+  </si>
+  <si>
+    <t>{'Answer:': 'Arthur Leigh Allen', 'Source:': 'https://en.wikipedia.org/wiki/Zodiac_Killer', 'Premise of the Question:': "The Zodiac Killer's real name was Arthur Leigh Allen, a former elementary school teacher and convicted sex offender who died in 1992. This is the most likely suspect identified by authorities, although the case remains open and the identity of the killer is still a mystery."}</t>
   </si>
 </sst>
 </file>
@@ -578,7 +573,7 @@
         <v>27</v>
       </c>
       <c r="F2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G2" t="s">
         <v>27</v>
@@ -587,10 +582,16 @@
         <v>-1</v>
       </c>
       <c r="I2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J2" t="s">
-        <v>38</v>
+        <v>36</v>
+      </c>
+      <c r="K2" t="s">
+        <v>41</v>
+      </c>
+      <c r="L2" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -610,7 +611,7 @@
         <v>28</v>
       </c>
       <c r="F3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G3" t="s">
         <v>28</v>
@@ -619,10 +620,16 @@
         <v>-1</v>
       </c>
       <c r="I3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J3" t="s">
-        <v>39</v>
+        <v>37</v>
+      </c>
+      <c r="K3" t="s">
+        <v>42</v>
+      </c>
+      <c r="L3" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -642,7 +649,7 @@
         <v>29</v>
       </c>
       <c r="F4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G4" t="s">
         <v>29</v>
@@ -651,10 +658,16 @@
         <v>-1</v>
       </c>
       <c r="I4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J4" t="s">
-        <v>40</v>
+        <v>38</v>
+      </c>
+      <c r="K4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -671,22 +684,28 @@
         <v>25</v>
       </c>
       <c r="E5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" t="s">
         <v>30</v>
       </c>
-      <c r="F5" t="s">
-        <v>32</v>
-      </c>
       <c r="G5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H5">
         <v>-1</v>
       </c>
       <c r="I5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J5" t="s">
-        <v>41</v>
+        <v>39</v>
+      </c>
+      <c r="K5" t="s">
+        <v>39</v>
+      </c>
+      <c r="L5" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -703,22 +722,28 @@
         <v>26</v>
       </c>
       <c r="E6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H6">
         <v>-1</v>
       </c>
       <c r="I6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J6" t="s">
-        <v>42</v>
+        <v>40</v>
+      </c>
+      <c r="K6" t="s">
+        <v>40</v>
+      </c>
+      <c r="L6" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>